<commit_message>
Calculate fraction of final sampling volume represented by tubing
Revised design has long tubing between canisters and 3-way valves at
sampling point. Internal volume of tube depends on tube diameter and
length. Calculations show even a 30 ft length of standard 1/4" tubing
has an internal volume representing less than 1% of the final sample
volume at 10% safety margin (approx 14L).
</commit_message>
<xml_diff>
--- a/engr/calculations.xlsx
+++ b/engr/calculations.xlsx
@@ -496,7 +496,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage of filled canister volume represented by volume in sampling tube</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -522,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -548,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A28" authorId="1" shapeId="0">
+    <comment ref="A30" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -572,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="1" shapeId="0">
+    <comment ref="A31" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -596,7 +620,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B29" authorId="1" shapeId="0">
+    <comment ref="B31" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -839,7 +863,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="199">
   <si>
     <t>Running power</t>
   </si>
@@ -1490,6 +1514,18 @@
   </si>
   <si>
     <t>Target design pressure</t>
+  </si>
+  <si>
+    <t>Tubing volume</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>Unit conversion: mL/in^3</t>
+  </si>
+  <si>
+    <t>Tubing volume fraction</t>
   </si>
 </sst>
 </file>
@@ -1726,7 +1762,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1904,6 +1940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1911,6 +1948,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1919,34 +1957,10 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="4"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
       </font>
       <fill>
         <patternFill>
@@ -2316,7 +2330,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2413,7 +2427,7 @@
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2513,7 +2527,7 @@
         <v>166</v>
       </c>
       <c r="B11" s="30">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>165</v>
@@ -2560,7 +2574,7 @@
       </c>
       <c r="B17" s="34">
         <f>B8*(0.528-B9)*1000/(B14*B16*60*B11)</f>
-        <v>10.334568491116546</v>
+        <v>7.7509263683374092</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>72</v>
@@ -2577,10 +2591,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2674,39 +2688,39 @@
         <v>ºF</v>
       </c>
       <c r="E3" s="39">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F3" s="40">
         <f>E3*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>37.649481131227979</v>
+        <v>34.226801028389069</v>
       </c>
       <c r="G3" s="41">
         <f>$B$15/(F3*$B$44)</f>
-        <v>0.16190668095716548</v>
+        <v>0.17809734905288202</v>
       </c>
       <c r="H3" s="42">
         <f t="shared" ref="H3:H31" si="0">G3*1000/100</f>
-        <v>1.6190668095716549</v>
+        <v>1.7809734905288201</v>
       </c>
       <c r="I3" s="42">
         <f t="shared" ref="I3:I21" si="1">G3*1000/50</f>
-        <v>3.2381336191433099</v>
+        <v>3.5619469810576403</v>
       </c>
       <c r="J3" s="40">
         <f>$B$21*F3*$B$14/($B$22*$B$40)</f>
-        <v>1851.1071970037769</v>
+        <v>1682.8247245488883</v>
       </c>
       <c r="K3" s="43">
         <f t="shared" ref="K3:K31" si="2">0.316/J3^0.25</f>
-        <v>4.8175828294676787E-2</v>
+        <v>4.9337525239560233E-2</v>
       </c>
       <c r="L3" s="41">
         <f>K3*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>2.0971255907323441</v>
+        <v>2.1476950251982969</v>
       </c>
       <c r="M3" s="41">
-        <f t="shared" ref="M3:M21" si="3">100*(2*6/1000)/E3</f>
-        <v>1.0909090909090908</v>
+        <f>100*(2*6/1000)/E3</f>
+        <v>1.2</v>
       </c>
       <c r="O3" s="35" t="str">
         <f>IF($J3&lt;$B$17," ",$L3)</f>
@@ -2727,83 +2741,83 @@
         <v>mbar</v>
       </c>
       <c r="E4" s="39">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="40">
         <f>E4*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>41.072161234066883</v>
+        <v>51.3402015425836</v>
       </c>
       <c r="G4" s="41">
         <f>$B$15/(F4*$B$44)</f>
-        <v>0.14841445754406835</v>
+        <v>0.11873156603525468</v>
       </c>
       <c r="H4" s="42">
         <f t="shared" si="0"/>
-        <v>1.4841445754406835</v>
+        <v>1.1873156603525468</v>
       </c>
       <c r="I4" s="42">
         <f t="shared" si="1"/>
-        <v>2.9682891508813669</v>
+        <v>2.3746313207050935</v>
       </c>
       <c r="J4" s="40">
         <f>$B$21*F4*$B$14/($B$22*$B$40)</f>
-        <v>2019.3896694586658</v>
+        <v>2524.237086823332</v>
       </c>
       <c r="K4" s="43">
         <f t="shared" si="2"/>
-        <v>4.7139182875338852E-2</v>
+        <v>4.4581486659617912E-2</v>
       </c>
       <c r="L4" s="41">
         <f>K4*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>2.0519997316788885</v>
+        <v>1.9406615279120769</v>
       </c>
       <c r="M4" s="41">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>100*(2*6/1000)/E4</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="O4" s="35" t="str">
-        <f t="shared" ref="O4:O31" si="4">IF($J4&lt;$B$17," ",$L4)</f>
+        <f>IF($J4&lt;$B$17," ",$L4)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E5" s="39">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="40">
         <f>E5*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>44.494841336905786</v>
+        <v>68.453602056778138</v>
       </c>
       <c r="G5" s="41">
         <f>$B$15/(F5*$B$44)</f>
-        <v>0.13699796080990928</v>
+        <v>8.904867452644101E-2</v>
       </c>
       <c r="H5" s="42">
         <f t="shared" si="0"/>
-        <v>1.3699796080990927</v>
+        <v>0.89048674526441007</v>
       </c>
       <c r="I5" s="42">
         <f t="shared" si="1"/>
-        <v>2.7399592161981854</v>
+        <v>1.7809734905288201</v>
       </c>
       <c r="J5" s="40">
         <f>$B$21*F5*$B$14/($B$22*$B$40)</f>
-        <v>2187.6721419135547</v>
+        <v>3365.6494490977766</v>
       </c>
       <c r="K5" s="43">
         <f t="shared" si="2"/>
-        <v>4.6205271182628696E-2</v>
+        <v>4.1487748111435852E-2</v>
       </c>
       <c r="L5" s="41">
         <f>K5*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>2.011345939526382</v>
+        <v>1.8059890477474829</v>
       </c>
       <c r="M5" s="41">
-        <f t="shared" si="3"/>
-        <v>0.92307692307692302</v>
+        <f>100*(2*6/1000)/E5</f>
+        <v>0.6</v>
       </c>
       <c r="O5" s="35" t="str">
-        <f t="shared" si="4"/>
+        <f>IF($J5&lt;$B$17," ",$L5)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2812,43 +2826,43 @@
         <v>48</v>
       </c>
       <c r="E6" s="39">
-        <v>1.4</v>
+        <v>2.5</v>
       </c>
       <c r="F6" s="40">
         <f>E6*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>47.917521439744689</v>
+        <v>85.567002570972676</v>
       </c>
       <c r="G6" s="41">
         <f>$B$15/(F6*$B$44)</f>
-        <v>0.12721239218063005</v>
+        <v>7.1238939621152811E-2</v>
       </c>
       <c r="H6" s="42">
         <f t="shared" si="0"/>
-        <v>1.2721239218063005</v>
+        <v>0.71238939621152808</v>
       </c>
       <c r="I6" s="42">
         <f t="shared" si="1"/>
-        <v>2.544247843612601</v>
+        <v>1.4247787924230562</v>
       </c>
       <c r="J6" s="40">
         <f>$B$21*F6*$B$14/($B$22*$B$40)</f>
-        <v>2355.9546143684433</v>
+        <v>4207.0618113722203</v>
       </c>
       <c r="K6" s="43">
         <f t="shared" si="2"/>
-        <v>4.535710766571046E-2</v>
+        <v>3.9236689652827825E-2</v>
       </c>
       <c r="L6" s="41">
         <f>K6*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.9744248220403473</v>
+        <v>1.7079989878588189</v>
       </c>
       <c r="M6" s="41">
-        <f t="shared" si="3"/>
-        <v>0.85714285714285721</v>
-      </c>
-      <c r="O6" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E6</f>
+        <v>0.48</v>
+      </c>
+      <c r="O6" s="35">
+        <f>IF($J6&lt;$B$17," ",$L6)</f>
+        <v>1.7079989878588189</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -2862,43 +2876,43 @@
         <v>190</v>
       </c>
       <c r="E7" s="39">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="40">
         <f>E7*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>51.3402015425836</v>
+        <v>102.6804030851672</v>
       </c>
       <c r="G7" s="41">
         <f>$B$15/(F7*$B$44)</f>
-        <v>0.11873156603525468</v>
+        <v>5.9365783017627342E-2</v>
       </c>
       <c r="H7" s="42">
         <f t="shared" si="0"/>
-        <v>1.1873156603525468</v>
+        <v>0.59365783017627338</v>
       </c>
       <c r="I7" s="42">
         <f t="shared" si="1"/>
-        <v>2.3746313207050935</v>
+        <v>1.1873156603525468</v>
       </c>
       <c r="J7" s="40">
         <f>$B$21*F7*$B$14/($B$22*$B$40)</f>
-        <v>2524.237086823332</v>
+        <v>5048.474173646664</v>
       </c>
       <c r="K7" s="43">
         <f t="shared" si="2"/>
-        <v>4.4581486659617912E-2</v>
+        <v>3.7488412318754001E-2</v>
       </c>
       <c r="L7" s="41">
         <f>K7*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.9406615279120769</v>
+        <v>1.6318953220420618</v>
       </c>
       <c r="M7" s="41">
-        <f t="shared" si="3"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="O7" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E7</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="O7" s="35">
+        <f>IF($J7&lt;$B$17," ",$L7)</f>
+        <v>1.6318953220420618</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -2909,43 +2923,43 @@
         <v>144</v>
       </c>
       <c r="E8" s="39">
-        <v>1.6</v>
+        <v>3.5</v>
       </c>
       <c r="F8" s="40">
         <f>E8*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>54.76288164542251</v>
+        <v>119.79380359936174</v>
       </c>
       <c r="G8" s="41">
         <f>$B$15/(F8*$B$44)</f>
-        <v>0.11131084315805127</v>
+        <v>5.0884956872252009E-2</v>
       </c>
       <c r="H8" s="42">
         <f t="shared" si="0"/>
-        <v>1.1131084315805126</v>
+        <v>0.50884956872252007</v>
       </c>
       <c r="I8" s="42">
         <f t="shared" si="1"/>
-        <v>2.2262168631610253</v>
+        <v>1.0176991374450401</v>
       </c>
       <c r="J8" s="40">
         <f>$B$21*F8*$B$14/($B$22*$B$40)</f>
-        <v>2692.5195592782211</v>
+        <v>5889.8865359211077</v>
       </c>
       <c r="K8" s="43">
         <f t="shared" si="2"/>
-        <v>4.3867952637892817E-2</v>
+        <v>3.607118006807513E-2</v>
       </c>
       <c r="L8" s="41">
         <f>K8*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.9096009211765779</v>
+        <v>1.5702022671197815</v>
       </c>
       <c r="M8" s="41">
-        <f t="shared" si="3"/>
-        <v>0.74999999999999989</v>
-      </c>
-      <c r="O8" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E8</f>
+        <v>0.34285714285714286</v>
+      </c>
+      <c r="O8" s="35">
+        <f>IF($J8&lt;$B$17," ",$L8)</f>
+        <v>1.5702022671197815</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -2960,43 +2974,43 @@
         <v>138</v>
       </c>
       <c r="E9" s="39">
-        <v>1.7</v>
+        <v>4</v>
       </c>
       <c r="F9" s="40">
         <f>E9*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>58.185561748261414</v>
+        <v>136.90720411355628</v>
       </c>
       <c r="G9" s="41">
         <f>$B$15/(F9*$B$44)</f>
-        <v>0.10476314650169533</v>
+        <v>4.4524337263220505E-2</v>
       </c>
       <c r="H9" s="42">
         <f t="shared" si="0"/>
-        <v>1.0476314650169534</v>
+        <v>0.44524337263220504</v>
       </c>
       <c r="I9" s="42">
         <f t="shared" si="1"/>
-        <v>2.0952629300339067</v>
+        <v>0.89048674526441007</v>
       </c>
       <c r="J9" s="40">
         <f>$B$21*F9*$B$14/($B$22*$B$40)</f>
-        <v>2860.8020317331093</v>
+        <v>6731.2988981955532</v>
       </c>
       <c r="K9" s="43">
         <f t="shared" si="2"/>
-        <v>4.3208096202814267E-2</v>
+        <v>3.4886898663855477E-2</v>
       </c>
       <c r="L9" s="41">
         <f>K9*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.880876935202775</v>
+        <v>1.5186497162383281</v>
       </c>
       <c r="M9" s="41">
-        <f t="shared" si="3"/>
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="O9" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E9</f>
+        <v>0.3</v>
+      </c>
+      <c r="O9" s="35">
+        <f>IF($J9&lt;$B$17," ",$L9)</f>
+        <v>1.5186497162383281</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3011,43 +3025,43 @@
         <v>138</v>
       </c>
       <c r="E10" s="39">
-        <v>1.8</v>
+        <v>4.5</v>
       </c>
       <c r="F10" s="40">
         <f>E10*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>61.608241851100324</v>
+        <v>154.0206046277508</v>
       </c>
       <c r="G10" s="41">
         <f>$B$15/(F10*$B$44)</f>
-        <v>9.8942971696045573E-2</v>
+        <v>3.9577188678418231E-2</v>
       </c>
       <c r="H10" s="42">
         <f t="shared" si="0"/>
-        <v>0.98942971696045579</v>
+        <v>0.39577188678418229</v>
       </c>
       <c r="I10" s="42">
         <f t="shared" si="1"/>
-        <v>1.9788594339209116</v>
+        <v>0.79154377356836458</v>
       </c>
       <c r="J10" s="40">
         <f>$B$21*F10*$B$14/($B$22*$B$40)</f>
-        <v>3029.0845041879988</v>
+        <v>7572.711260469996</v>
       </c>
       <c r="K10" s="43">
         <f t="shared" si="2"/>
-        <v>4.2595060094687061E-2</v>
+        <v>3.3874604483378104E-2</v>
       </c>
       <c r="L10" s="41">
         <f>K10*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.854191068951907</v>
+        <v>1.4745838826787401</v>
       </c>
       <c r="M10" s="41">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O10" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E10</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="O10" s="35">
+        <f>IF($J10&lt;$B$17," ",$L10)</f>
+        <v>1.4745838826787401</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -3062,84 +3076,84 @@
         <v>138</v>
       </c>
       <c r="E11" s="39">
-        <v>1.9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="40">
         <f>E11*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>65.030921953939227</v>
+        <v>171.13400514194535</v>
       </c>
       <c r="G11" s="41">
         <f>$B$15/(F11*$B$44)</f>
-        <v>9.3735446869937913E-2</v>
+        <v>3.5619469810576405E-2</v>
       </c>
       <c r="H11" s="42">
         <f t="shared" si="0"/>
-        <v>0.93735446869937922</v>
+        <v>0.35619469810576404</v>
       </c>
       <c r="I11" s="42">
         <f t="shared" si="1"/>
-        <v>1.8747089373987584</v>
+        <v>0.71238939621152808</v>
       </c>
       <c r="J11" s="40">
         <f>$B$21*F11*$B$14/($B$22*$B$40)</f>
-        <v>3197.3669766428875</v>
+        <v>8414.1236227444406</v>
       </c>
       <c r="K11" s="43">
         <f t="shared" si="2"/>
-        <v>4.2023184631517101E-2</v>
+        <v>3.2993991675485425E-2</v>
       </c>
       <c r="L11" s="41">
         <f>K11*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.8292969527326712</v>
+        <v>1.4362502261474528</v>
       </c>
       <c r="M11" s="41">
-        <f t="shared" si="3"/>
-        <v>0.63157894736842102</v>
-      </c>
-      <c r="O11" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E11</f>
+        <v>0.24</v>
+      </c>
+      <c r="O11" s="35">
+        <f>IF($J11&lt;$B$17," ",$L11)</f>
+        <v>1.4362502261474528</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E12" s="39">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="F12" s="40">
         <f>E12*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>68.453602056778138</v>
+        <v>188.24740565613988</v>
       </c>
       <c r="G12" s="41">
         <f>$B$15/(F12*$B$44)</f>
-        <v>8.904867452644101E-2</v>
+        <v>3.2381336191433095E-2</v>
       </c>
       <c r="H12" s="42">
         <f t="shared" si="0"/>
-        <v>0.89048674526441007</v>
+        <v>0.32381336191433091</v>
       </c>
       <c r="I12" s="42">
         <f t="shared" si="1"/>
-        <v>1.7809734905288201</v>
+        <v>0.64762672382866182</v>
       </c>
       <c r="J12" s="40">
         <f>$B$21*F12*$B$14/($B$22*$B$40)</f>
-        <v>3365.6494490977766</v>
+        <v>9255.5359850188852</v>
       </c>
       <c r="K12" s="43">
         <f t="shared" si="2"/>
-        <v>4.1487748111435852E-2</v>
+        <v>3.2217118106273888E-2</v>
       </c>
       <c r="L12" s="41">
         <f>K12*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.8059890477474829</v>
+        <v>1.4024324071202066</v>
       </c>
       <c r="M12" s="41">
-        <f t="shared" si="3"/>
-        <v>0.6</v>
-      </c>
-      <c r="O12" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E12</f>
+        <v>0.21818181818181817</v>
+      </c>
+      <c r="O12" s="35">
+        <f>IF($J12&lt;$B$17," ",$L12)</f>
+        <v>1.4024324071202066</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -3147,281 +3161,281 @@
         <v>140</v>
       </c>
       <c r="E13" s="39">
-        <v>2.1</v>
+        <v>6</v>
       </c>
       <c r="F13" s="40">
         <f>E13*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>71.876282159617048</v>
+        <v>205.3608061703344</v>
       </c>
       <c r="G13" s="41">
         <f>$B$15/(F13*$B$44)</f>
-        <v>8.4808261453753336E-2</v>
+        <v>2.9682891508813671E-2</v>
       </c>
       <c r="H13" s="42">
         <f t="shared" si="0"/>
-        <v>0.84808261453753331</v>
+        <v>0.29682891508813669</v>
       </c>
       <c r="I13" s="42">
         <f t="shared" si="1"/>
-        <v>1.6961652290750666</v>
+        <v>0.59365783017627338</v>
       </c>
       <c r="J13" s="40">
         <f>$B$21*F13*$B$14/($B$22*$B$40)</f>
-        <v>3533.9319215526652</v>
+        <v>10096.948347293328</v>
       </c>
       <c r="K13" s="43">
         <f t="shared" si="2"/>
-        <v>4.0984773364683418E-2</v>
+        <v>3.152387153239343E-2</v>
       </c>
       <c r="L13" s="41">
         <f>K13*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.784094225172669</v>
+        <v>1.3722549263744759</v>
       </c>
       <c r="M13" s="41">
-        <f t="shared" si="3"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="O13" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E13</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="O13" s="35">
+        <f>IF($J13&lt;$B$17," ",$L13)</f>
+        <v>1.3722549263744759</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="71">
+      <c r="B14" s="72">
         <v>3.1E-2</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>138</v>
       </c>
       <c r="E14" s="39">
-        <v>2.2000000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="F14" s="40">
         <f>E14*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>75.298962262455959</v>
+        <v>222.47420668452895</v>
       </c>
       <c r="G14" s="41">
         <f>$B$15/(F14*$B$44)</f>
-        <v>8.0953340478582742E-2</v>
+        <v>2.7399592161981848E-2</v>
       </c>
       <c r="H14" s="42">
         <f t="shared" si="0"/>
-        <v>0.80953340478582747</v>
+        <v>0.27399592161981845</v>
       </c>
       <c r="I14" s="42">
         <f t="shared" si="1"/>
-        <v>1.6190668095716549</v>
+        <v>0.5479918432396369</v>
       </c>
       <c r="J14" s="40">
         <f>$B$21*F14*$B$14/($B$22*$B$40)</f>
-        <v>3702.2143940075539</v>
+        <v>10938.360709567774</v>
       </c>
       <c r="K14" s="43">
         <f t="shared" si="2"/>
-        <v>4.0510881314872176E-2</v>
+        <v>3.0899327142189396E-2</v>
       </c>
       <c r="L14" s="41">
         <f>K14*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.763465391583656</v>
+        <v>1.3450680970119608</v>
       </c>
       <c r="M14" s="41">
-        <f t="shared" si="3"/>
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="O14" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E14</f>
+        <v>0.1846153846153846</v>
+      </c>
+      <c r="O14" s="35">
+        <f>IF($J14&lt;$B$17," ",$L14)</f>
+        <v>1.3450680970119608</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="72">
         <v>20</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>136</v>
       </c>
       <c r="E15" s="39">
-        <v>2.2999999999999998</v>
+        <v>7</v>
       </c>
       <c r="F15" s="40">
         <f>E15*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>78.721642365294855</v>
+        <v>239.58760719872348</v>
       </c>
       <c r="G15" s="41">
         <f>$B$15/(F15*$B$44)</f>
-        <v>7.7433630022992195E-2</v>
+        <v>2.5442478436126004E-2</v>
       </c>
       <c r="H15" s="42">
         <f t="shared" si="0"/>
-        <v>0.77433630022992195</v>
+        <v>0.25442478436126004</v>
       </c>
       <c r="I15" s="42">
         <f t="shared" si="1"/>
-        <v>1.5486726004598439</v>
+        <v>0.50884956872252007</v>
       </c>
       <c r="J15" s="40">
         <f>$B$21*F15*$B$14/($B$22*$B$40)</f>
-        <v>3870.496866462443</v>
+        <v>11779.773071842215</v>
       </c>
       <c r="K15" s="43">
         <f t="shared" si="2"/>
-        <v>4.0063178550064631E-2</v>
+        <v>3.0332126013215627E-2</v>
       </c>
       <c r="L15" s="41">
         <f>K15*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.743976594849812</v>
+        <v>1.3203774576442797</v>
       </c>
       <c r="M15" s="41">
-        <f t="shared" si="3"/>
-        <v>0.52173913043478259</v>
-      </c>
-      <c r="O15" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E15</f>
+        <v>0.17142857142857143</v>
+      </c>
+      <c r="O15" s="35">
+        <f>IF($J15&lt;$B$17," ",$L15)</f>
+        <v>1.3203774576442797</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B16" s="72">
+      <c r="B16" s="73">
         <v>50</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>173</v>
       </c>
       <c r="E16" s="39">
-        <v>2.4</v>
+        <v>7.5</v>
       </c>
       <c r="F16" s="40">
         <f>E16*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>82.144322468133765</v>
+        <v>256.701007712918</v>
       </c>
       <c r="G16" s="41">
         <f>$B$15/(F16*$B$44)</f>
-        <v>7.4207228772034173E-2</v>
+        <v>2.374631320705094E-2</v>
       </c>
       <c r="H16" s="42">
         <f t="shared" si="0"/>
-        <v>0.74207228772034173</v>
+        <v>0.2374631320705094</v>
       </c>
       <c r="I16" s="42">
         <f t="shared" si="1"/>
-        <v>1.4841445754406835</v>
+        <v>0.47492626414101879</v>
       </c>
       <c r="J16" s="40">
         <f>$B$21*F16*$B$14/($B$22*$B$40)</f>
-        <v>4038.7793389173316</v>
+        <v>12621.185434116662</v>
       </c>
       <c r="K16" s="43">
         <f t="shared" si="2"/>
-        <v>3.9639169897861731E-2</v>
+        <v>2.9813436985055179E-2</v>
       </c>
       <c r="L16" s="41">
         <f>K16*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.7255192184703614</v>
+        <v>1.2977985820319318</v>
       </c>
       <c r="M16" s="41">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="O16" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> </v>
+        <f>100*(2*6/1000)/E16</f>
+        <v>0.16</v>
+      </c>
+      <c r="O16" s="35">
+        <f>IF($J16&lt;$B$17," ",$L16)</f>
+        <v>1.2977985820319318</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="B17" s="72">
+      <c r="B17" s="73">
         <v>4100</v>
       </c>
       <c r="E17" s="39">
-        <v>2.5</v>
+        <v>8</v>
       </c>
       <c r="F17" s="40">
         <f>E17*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>85.567002570972676</v>
+        <v>273.81440822711255</v>
       </c>
       <c r="G17" s="41">
         <f>$B$15/(F17*$B$44)</f>
-        <v>7.1238939621152811E-2</v>
+        <v>2.2262168631610253E-2</v>
       </c>
       <c r="H17" s="42">
         <f t="shared" si="0"/>
-        <v>0.71238939621152808</v>
+        <v>0.22262168631610252</v>
       </c>
       <c r="I17" s="42">
         <f t="shared" si="1"/>
-        <v>1.4247787924230562</v>
+        <v>0.44524337263220504</v>
       </c>
       <c r="J17" s="40">
         <f>$B$21*F17*$B$14/($B$22*$B$40)</f>
-        <v>4207.0618113722203</v>
+        <v>13462.597796391106</v>
       </c>
       <c r="K17" s="43">
         <f t="shared" si="2"/>
-        <v>3.9236689652827825E-2</v>
+        <v>2.9336268025755671E-2</v>
       </c>
       <c r="L17" s="41">
         <f>K17*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.7079989878588189</v>
+        <v>1.277027102410881</v>
       </c>
       <c r="M17" s="41">
-        <f t="shared" si="3"/>
-        <v>0.48</v>
+        <f>100*(2*6/1000)/E17</f>
+        <v>0.15</v>
       </c>
       <c r="O17" s="35">
-        <f t="shared" si="4"/>
-        <v>1.7079989878588189</v>
+        <f>IF($J17&lt;$B$17," ",$L17)</f>
+        <v>1.277027102410881</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E18" s="39">
-        <v>2.6</v>
+        <v>8.5</v>
       </c>
       <c r="F18" s="40">
         <f>E18*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>88.989682673811572</v>
+        <v>290.92780874130705</v>
       </c>
       <c r="G18" s="41">
         <f>$B$15/(F18*$B$44)</f>
-        <v>6.849898040495464E-2</v>
+        <v>2.0952629300339067E-2</v>
       </c>
       <c r="H18" s="42">
         <f t="shared" si="0"/>
-        <v>0.68498980404954635</v>
+        <v>0.20952629300339065</v>
       </c>
       <c r="I18" s="42">
         <f t="shared" si="1"/>
-        <v>1.3699796080990927</v>
+        <v>0.4190525860067813</v>
       </c>
       <c r="J18" s="40">
         <f>$B$21*F18*$B$14/($B$22*$B$40)</f>
-        <v>4375.3442838271094</v>
+        <v>14304.010158665547</v>
       </c>
       <c r="K18" s="43">
         <f t="shared" si="2"/>
-        <v>3.8853846903298218E-2</v>
+        <v>2.8894995432120596E-2</v>
       </c>
       <c r="L18" s="41">
         <f>K18*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6913335903828486</v>
+        <v>1.2578182152706219</v>
       </c>
       <c r="M18" s="41">
-        <f t="shared" si="3"/>
-        <v>0.46153846153846151</v>
+        <f>100*(2*6/1000)/E18</f>
+        <v>0.14117647058823529</v>
       </c>
       <c r="O18" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6913335903828486</v>
+        <f>IF($J18&lt;$B$17," ",$L18)</f>
+        <v>1.2578182152706219</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -3429,43 +3443,43 @@
         <v>117</v>
       </c>
       <c r="E19" s="39">
-        <v>2.7</v>
+        <v>9</v>
       </c>
       <c r="F19" s="40">
         <f>E19*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>92.412362776650482</v>
+        <v>308.0412092555016</v>
       </c>
       <c r="G19" s="41">
         <f>$B$15/(F19*$B$44)</f>
-        <v>6.5961981130697039E-2</v>
+        <v>1.9788594339209115E-2</v>
       </c>
       <c r="H19" s="42">
         <f t="shared" si="0"/>
-        <v>0.65961981130697045</v>
+        <v>0.19788594339209115</v>
       </c>
       <c r="I19" s="42">
         <f t="shared" si="1"/>
-        <v>1.3192396226139409</v>
+        <v>0.39577188678418229</v>
       </c>
       <c r="J19" s="40">
         <f>$B$21*F19*$B$14/($B$22*$B$40)</f>
-        <v>4543.6267562819985</v>
+        <v>15145.422520939992</v>
       </c>
       <c r="K19" s="43">
         <f t="shared" si="2"/>
-        <v>3.8488981645440984E-2</v>
+        <v>2.8485033478210058E-2</v>
       </c>
       <c r="L19" s="41">
         <f>K19*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6754507649804236</v>
+        <v>1.2399723009354566</v>
       </c>
       <c r="M19" s="41">
-        <f t="shared" si="3"/>
-        <v>0.44444444444444442</v>
+        <f>100*(2*6/1000)/E19</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="O19" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6754507649804236</v>
+        <f>IF($J19&lt;$B$17," ",$L19)</f>
+        <v>1.2399723009354566</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -3480,43 +3494,43 @@
         <v>115</v>
       </c>
       <c r="E20" s="39">
-        <v>2.8</v>
+        <v>9.5</v>
       </c>
       <c r="F20" s="40">
         <f>E20*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>95.835042879489379</v>
+        <v>325.15460976969615</v>
       </c>
       <c r="G20" s="41">
         <f>$B$15/(F20*$B$44)</f>
-        <v>6.3606196090315023E-2</v>
+        <v>1.8747089373987582E-2</v>
       </c>
       <c r="H20" s="42">
         <f t="shared" si="0"/>
-        <v>0.63606196090315026</v>
+        <v>0.1874708937398758</v>
       </c>
       <c r="I20" s="42">
         <f t="shared" si="1"/>
-        <v>1.2721239218063005</v>
+        <v>0.3749417874797516</v>
       </c>
       <c r="J20" s="40">
         <f>$B$21*F20*$B$14/($B$22*$B$40)</f>
-        <v>4711.9092287368867</v>
+        <v>15986.834883214438</v>
       </c>
       <c r="K20" s="43">
         <f t="shared" si="2"/>
-        <v>3.8140629242372701E-2</v>
+        <v>2.8102597306561231E-2</v>
       </c>
       <c r="L20" s="41">
         <f>K20*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6602867550416818</v>
+        <v>1.2233246020628858</v>
       </c>
       <c r="M20" s="41">
-        <f t="shared" si="3"/>
-        <v>0.4285714285714286</v>
+        <f>100*(2*6/1000)/E20</f>
+        <v>0.12631578947368421</v>
       </c>
       <c r="O20" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6602867550416818</v>
+        <f>IF($J20&lt;$B$17," ",$L20)</f>
+        <v>1.2233246020628858</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -3531,43 +3545,43 @@
         <v>113</v>
       </c>
       <c r="E21" s="39">
-        <v>2.9</v>
+        <v>10</v>
       </c>
       <c r="F21" s="40">
         <f>E21*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>99.257722982328303</v>
+        <v>342.2680102838907</v>
       </c>
       <c r="G21" s="41">
         <f>$B$15/(F21*$B$44)</f>
-        <v>6.1412878983752424E-2</v>
+        <v>1.7809734905288203E-2</v>
       </c>
       <c r="H21" s="42">
         <f t="shared" si="0"/>
-        <v>0.61412878983752417</v>
+        <v>0.17809734905288202</v>
       </c>
       <c r="I21" s="42">
         <f t="shared" si="1"/>
-        <v>1.2282575796750483</v>
+        <v>0.35619469810576404</v>
       </c>
       <c r="J21" s="40">
         <f>$B$21*F21*$B$14/($B$22*$B$40)</f>
-        <v>4880.1917011917758</v>
+        <v>16828.247245488881</v>
       </c>
       <c r="K21" s="43">
         <f t="shared" si="2"/>
-        <v>3.7807491405126334E-2</v>
+        <v>2.7744529324826593E-2</v>
       </c>
       <c r="L21" s="41">
         <f>K21*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6457850451913132</v>
+        <v>1.2077376665747301</v>
       </c>
       <c r="M21" s="41">
-        <f t="shared" si="3"/>
-        <v>0.41379310344827586</v>
+        <f>100*(2*6/1000)/E21</f>
+        <v>0.12</v>
       </c>
       <c r="O21" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6457850451913132</v>
+        <f>IF($J21&lt;$B$17," ",$L21)</f>
+        <v>1.2077376665747301</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -3582,43 +3596,43 @@
         <v>111</v>
       </c>
       <c r="E22" s="39">
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="F22" s="40">
         <f>E22*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>102.6804030851672</v>
+        <v>359.3814107980852</v>
       </c>
       <c r="G22" s="41">
         <f>$B$15/(F22*$B$44)</f>
-        <v>5.9365783017627342E-2</v>
+        <v>1.6961652290750671E-2</v>
       </c>
       <c r="H22" s="42">
         <f t="shared" si="0"/>
-        <v>0.59365783017627338</v>
+        <v>0.1696165229075067</v>
       </c>
       <c r="I22" s="42">
-        <f t="shared" ref="I22:I31" si="5">G22*1000/50</f>
-        <v>1.1873156603525468</v>
+        <f t="shared" ref="I22:I31" si="3">G22*1000/50</f>
+        <v>0.3392330458150134</v>
       </c>
       <c r="J22" s="40">
         <f>$B$21*F22*$B$14/($B$22*$B$40)</f>
-        <v>5048.474173646664</v>
+        <v>17669.659607763326</v>
       </c>
       <c r="K22" s="43">
         <f t="shared" si="2"/>
-        <v>3.7488412318754001E-2</v>
+        <v>2.7408169839287927E-2</v>
       </c>
       <c r="L22" s="41">
         <f>K22*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6318953220420618</v>
+        <v>1.1930957162486442</v>
       </c>
       <c r="M22" s="41">
-        <f t="shared" ref="M22:M31" si="6">100*(2*6/1000)/E22</f>
-        <v>0.39999999999999997</v>
+        <f>100*(2*6/1000)/E22</f>
+        <v>0.11428571428571428</v>
       </c>
       <c r="O22" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6318953220420618</v>
+        <f>IF($J22&lt;$B$17," ",$L22)</f>
+        <v>1.1930957162486442</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -3633,431 +3647,448 @@
         <v>109</v>
       </c>
       <c r="E23" s="39">
-        <v>3.1</v>
+        <v>11</v>
       </c>
       <c r="F23" s="40">
         <f>E23*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>106.10308318800611</v>
+        <v>376.49481131227975</v>
       </c>
       <c r="G23" s="41">
         <f>$B$15/(F23*$B$44)</f>
-        <v>5.7450757758994206E-2</v>
+        <v>1.6190668095716548E-2</v>
       </c>
       <c r="H23" s="42">
         <f t="shared" si="0"/>
-        <v>0.57450757758994209</v>
+        <v>0.16190668095716546</v>
       </c>
       <c r="I23" s="42">
-        <f t="shared" si="5"/>
-        <v>1.1490151551798842</v>
+        <f t="shared" si="3"/>
+        <v>0.32381336191433091</v>
       </c>
       <c r="J23" s="40">
         <f>$B$21*F23*$B$14/($B$22*$B$40)</f>
-        <v>5216.7566461015531</v>
+        <v>18511.07197003777</v>
       </c>
       <c r="K23" s="43">
         <f t="shared" si="2"/>
-        <v>3.7182358862969465E-2</v>
+        <v>2.7091259125371251E-2</v>
       </c>
       <c r="L23" s="41">
         <f>K23*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6185726131862448</v>
+        <v>1.1793003837830196</v>
       </c>
       <c r="M23" s="41">
-        <f t="shared" si="6"/>
-        <v>0.38709677419354838</v>
+        <f>100*(2*6/1000)/E23</f>
+        <v>0.10909090909090909</v>
       </c>
       <c r="O23" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6185726131862448</v>
+        <f>IF($J23&lt;$B$17," ",$L23)</f>
+        <v>1.1793003837830196</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="71">
+        <f>$B$15*$B$23*$B$43*$B$46</f>
+        <v>2.9684221296677897</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="39">
+        <v>11.5</v>
+      </c>
+      <c r="F24" s="40">
+        <f>E24*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>393.60821182647425</v>
+      </c>
+      <c r="G24" s="41">
+        <f>$B$15/(F24*$B$44)</f>
+        <v>1.5486726004598439E-2</v>
+      </c>
+      <c r="H24" s="42">
+        <f t="shared" si="0"/>
+        <v>0.15486726004598439</v>
+      </c>
+      <c r="I24" s="42">
+        <f t="shared" si="3"/>
+        <v>0.30973452009196878</v>
+      </c>
+      <c r="J24" s="40">
+        <f>$B$21*F24*$B$14/($B$22*$B$40)</f>
+        <v>19352.484332312211</v>
+      </c>
+      <c r="K24" s="43">
+        <f t="shared" si="2"/>
+        <v>2.6791862241895063E-2</v>
+      </c>
+      <c r="L24" s="41">
+        <f>K24*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1662674399116051</v>
+      </c>
+      <c r="M24" s="41">
+        <f>100*(2*6/1000)/E24</f>
+        <v>0.10434782608695652</v>
+      </c>
+      <c r="O24" s="35">
+        <f>IF($J24&lt;$B$17," ",$L24)</f>
+        <v>1.1662674399116051</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="75">
+        <f>(B24/B42)/(Canisters!B8*(0.528-Canisters!B9))</f>
+        <v>2.1016865828857187E-4</v>
+      </c>
+      <c r="E25" s="39">
+        <v>12</v>
+      </c>
+      <c r="F25" s="40">
+        <f>E25*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>410.7216123406688</v>
+      </c>
+      <c r="G25" s="41">
+        <f>$B$15/(F25*$B$44)</f>
+        <v>1.4841445754406836E-2</v>
+      </c>
+      <c r="H25" s="42">
+        <f t="shared" si="0"/>
+        <v>0.14841445754406835</v>
+      </c>
+      <c r="I25" s="42">
+        <f t="shared" si="3"/>
+        <v>0.29682891508813669</v>
+      </c>
+      <c r="J25" s="40">
+        <f>$B$21*F25*$B$14/($B$22*$B$40)</f>
+        <v>20193.896694586656</v>
+      </c>
+      <c r="K25" s="43">
+        <f t="shared" si="2"/>
+        <v>2.6508310566508257E-2</v>
+      </c>
+      <c r="L25" s="41">
+        <f>K25*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1539242484025469</v>
+      </c>
+      <c r="M25" s="41">
+        <f>100*(2*6/1000)/E25</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="O25" s="35">
+        <f>IF($J25&lt;$B$17," ",$L25)</f>
+        <v>1.1539242484025469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B26" s="51">
         <f>-1*B7*B39</f>
         <v>-482.58</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C26" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="E24" s="39">
-        <v>3.2</v>
-      </c>
-      <c r="F24" s="40">
-        <f>E24*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>109.52576329084502</v>
-      </c>
-      <c r="G24" s="41">
-        <f>$B$15/(F24*$B$44)</f>
-        <v>5.5655421579025637E-2</v>
-      </c>
-      <c r="H24" s="42">
+      <c r="E26" s="39">
+        <v>12.5</v>
+      </c>
+      <c r="F26" s="40">
+        <f>E26*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>427.83501285486329</v>
+      </c>
+      <c r="G26" s="41">
+        <f>$B$15/(F26*$B$44)</f>
+        <v>1.4247787924230565E-2</v>
+      </c>
+      <c r="H26" s="42">
         <f t="shared" si="0"/>
-        <v>0.55655421579025632</v>
-      </c>
-      <c r="I24" s="42">
-        <f t="shared" si="5"/>
-        <v>1.1131084315805126</v>
-      </c>
-      <c r="J24" s="40">
-        <f>$B$21*F24*$B$14/($B$22*$B$40)</f>
-        <v>5385.0391185564422</v>
-      </c>
-      <c r="K24" s="43">
+        <v>0.14247787924230565</v>
+      </c>
+      <c r="I26" s="42">
+        <f t="shared" si="3"/>
+        <v>0.2849557584846113</v>
+      </c>
+      <c r="J26" s="40">
+        <f>$B$21*F26*$B$14/($B$22*$B$40)</f>
+        <v>21035.309056861101</v>
+      </c>
+      <c r="K26" s="43">
         <f t="shared" si="2"/>
-        <v>3.6888404117723796E-2</v>
-      </c>
-      <c r="L24" s="41">
-        <f>K24*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.6057765691825754</v>
-      </c>
-      <c r="M24" s="41">
-        <f t="shared" si="6"/>
-        <v>0.37499999999999994</v>
-      </c>
-      <c r="O24" s="35">
-        <f t="shared" si="4"/>
-        <v>1.6057765691825754</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="50" t="s">
+        <v>2.6239155804697292E-2</v>
+      </c>
+      <c r="L26" s="41">
+        <f>K26*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1422077640401258</v>
+      </c>
+      <c r="M26" s="41">
+        <f>100*(2*6/1000)/E26</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="O26" s="35">
+        <f>IF($J26&lt;$B$17," ",$L26)</f>
+        <v>1.1422077640401258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="B25" s="51">
+      <c r="B27" s="51">
         <f>-1*(1-$B$37)*$B$4-$B$16</f>
         <v>-485.65599999999995</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C27" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="E25" s="39">
-        <v>3.3</v>
-      </c>
-      <c r="F25" s="40">
-        <f>E25*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>112.94844339368392</v>
-      </c>
-      <c r="G25" s="41">
-        <f>$B$15/(F25*$B$44)</f>
-        <v>5.3968893652388494E-2</v>
-      </c>
-      <c r="H25" s="42">
+      <c r="E27" s="39">
+        <v>13</v>
+      </c>
+      <c r="F27" s="40">
+        <f>E27*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>444.9484133690579</v>
+      </c>
+      <c r="G27" s="41">
+        <f>$B$15/(F27*$B$44)</f>
+        <v>1.3699796080990924E-2</v>
+      </c>
+      <c r="H27" s="42">
         <f t="shared" si="0"/>
-        <v>0.53968893652388494</v>
-      </c>
-      <c r="I25" s="42">
-        <f t="shared" si="5"/>
-        <v>1.0793778730477699</v>
-      </c>
-      <c r="J25" s="40">
-        <f>$B$21*F25*$B$14/($B$22*$B$40)</f>
-        <v>5553.3215910113304</v>
-      </c>
-      <c r="K25" s="43">
+        <v>0.13699796080990922</v>
+      </c>
+      <c r="I27" s="42">
+        <f t="shared" si="3"/>
+        <v>0.27399592161981845</v>
+      </c>
+      <c r="J27" s="40">
+        <f>$B$21*F27*$B$14/($B$22*$B$40)</f>
+        <v>21876.721419135549</v>
+      </c>
+      <c r="K27" s="43">
         <f t="shared" si="2"/>
-        <v>3.6605713524119135E-2</v>
-      </c>
-      <c r="L25" s="41">
-        <f>K25*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5934708611316117</v>
-      </c>
-      <c r="M25" s="41">
-        <f t="shared" si="6"/>
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="O25" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5934708611316117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
+        <v>2.5983133427618869E-2</v>
+      </c>
+      <c r="L27" s="41">
+        <f>K27*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1310629410494935</v>
+      </c>
+      <c r="M27" s="41">
+        <f>100*(2*6/1000)/E27</f>
+        <v>9.2307692307692299E-2</v>
+      </c>
+      <c r="O27" s="35">
+        <f>IF($J27&lt;$B$17," ",$L27)</f>
+        <v>1.1310629410494935</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B28" s="51">
         <f>$B$4*$B$37</f>
         <v>487.34400000000005</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C28" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="E26" s="39">
-        <v>3.4</v>
-      </c>
-      <c r="F26" s="40">
-        <f>E26*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>116.37112349652283</v>
-      </c>
-      <c r="G26" s="41">
-        <f>$B$15/(F26*$B$44)</f>
-        <v>5.2381573250847663E-2</v>
-      </c>
-      <c r="H26" s="42">
+      <c r="E28" s="39">
+        <v>13.5</v>
+      </c>
+      <c r="F28" s="40">
+        <f>E28*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>462.0618138832524</v>
+      </c>
+      <c r="G28" s="41">
+        <f>$B$15/(F28*$B$44)</f>
+        <v>1.319239622613941E-2</v>
+      </c>
+      <c r="H28" s="42">
         <f t="shared" si="0"/>
-        <v>0.52381573250847668</v>
-      </c>
-      <c r="I26" s="42">
-        <f t="shared" si="5"/>
-        <v>1.0476314650169534</v>
-      </c>
-      <c r="J26" s="40">
-        <f>$B$21*F26*$B$14/($B$22*$B$40)</f>
-        <v>5721.6040634662186</v>
-      </c>
-      <c r="K26" s="43">
+        <v>0.13192396226139411</v>
+      </c>
+      <c r="I28" s="42">
+        <f t="shared" si="3"/>
+        <v>0.26384792452278821</v>
+      </c>
+      <c r="J28" s="40">
+        <f>$B$21*F28*$B$14/($B$22*$B$40)</f>
+        <v>22718.13378140999</v>
+      </c>
+      <c r="K28" s="43">
         <f t="shared" si="2"/>
-        <v>3.633353320688415E-2</v>
-      </c>
-      <c r="L26" s="41">
-        <f>K26*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5816226723454063</v>
-      </c>
-      <c r="M26" s="41">
-        <f t="shared" si="6"/>
-        <v>0.35294117647058826</v>
-      </c>
-      <c r="O26" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5816226723454063</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+        <v>2.5739133323804106E-2</v>
+      </c>
+      <c r="L28" s="41">
+        <f>K28*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1204414555459878</v>
+      </c>
+      <c r="M28" s="41">
+        <f>100*(2*6/1000)/E28</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="O28" s="35">
+        <f>IF($J28&lt;$B$17," ",$L28)</f>
+        <v>1.1204414555459878</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="B27" s="51">
-        <f>$B$4+MIN($B$24:$B$25)-MAX($O$3:$O$31)</f>
+      <c r="B29" s="51">
+        <f>$B$4+MIN($B$26:$B$27)-MAX($O$3:$O$31)</f>
         <v>435.63600101214121</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C29" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="E27" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="F27" s="40">
-        <f>E27*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>119.79380359936174</v>
-      </c>
-      <c r="G27" s="41">
-        <f>$B$15/(F27*$B$44)</f>
-        <v>5.0884956872252009E-2</v>
-      </c>
-      <c r="H27" s="42">
+      <c r="E29" s="39">
+        <v>14</v>
+      </c>
+      <c r="F29" s="40">
+        <f>E29*$B$40^2/($B$23*$B$41*$B$42)</f>
+        <v>479.17521439744695</v>
+      </c>
+      <c r="G29" s="41">
+        <f>$B$15/(F29*$B$44)</f>
+        <v>1.2721239218063002E-2</v>
+      </c>
+      <c r="H29" s="42">
         <f t="shared" si="0"/>
-        <v>0.50884956872252007</v>
-      </c>
-      <c r="I27" s="42">
-        <f t="shared" si="5"/>
-        <v>1.0176991374450401</v>
-      </c>
-      <c r="J27" s="40">
-        <f>$B$21*F27*$B$14/($B$22*$B$40)</f>
-        <v>5889.8865359211077</v>
-      </c>
-      <c r="K27" s="43">
+        <v>0.12721239218063002</v>
+      </c>
+      <c r="I29" s="42">
+        <f t="shared" si="3"/>
+        <v>0.25442478436126004</v>
+      </c>
+      <c r="J29" s="40">
+        <f>$B$21*F29*$B$14/($B$22*$B$40)</f>
+        <v>23559.546143684431</v>
+      </c>
+      <c r="K29" s="43">
         <f t="shared" si="2"/>
-        <v>3.607118006807513E-2</v>
-      </c>
-      <c r="L27" s="41">
-        <f>K27*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5702022671197815</v>
-      </c>
-      <c r="M27" s="41">
-        <f t="shared" si="6"/>
-        <v>0.34285714285714286</v>
-      </c>
-      <c r="O27" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5702022671197815</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
+        <v>2.5506176031536966E-2</v>
+      </c>
+      <c r="L29" s="41">
+        <f>K29*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
+        <v>1.1103006709148884</v>
+      </c>
+      <c r="M29" s="41">
+        <f>100*(2*6/1000)/E29</f>
+        <v>8.5714285714285715E-2</v>
+      </c>
+      <c r="O29" s="35">
+        <f>IF($J29&lt;$B$17," ",$L29)</f>
+        <v>1.1103006709148884</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B28" s="51">
+      <c r="B30" s="51">
         <f>$B$4*($B$37-Canisters!B9)</f>
         <v>395.04400000000004</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C30" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="E28" s="39">
-        <v>3.6</v>
-      </c>
-      <c r="F28" s="40">
-        <f>E28*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>123.21648370220065</v>
-      </c>
-      <c r="G28" s="41">
-        <f>$B$15/(F28*$B$44)</f>
-        <v>4.9471485848022786E-2</v>
-      </c>
-      <c r="H28" s="42">
-        <f t="shared" si="0"/>
-        <v>0.49471485848022789</v>
-      </c>
-      <c r="I28" s="42">
-        <f t="shared" si="5"/>
-        <v>0.98942971696045579</v>
-      </c>
-      <c r="J28" s="40">
-        <f>$B$21*F28*$B$14/($B$22*$B$40)</f>
-        <v>6058.1690083759977</v>
-      </c>
-      <c r="K28" s="43">
-        <f t="shared" si="2"/>
-        <v>3.5818033341138901E-2</v>
-      </c>
-      <c r="L28" s="41">
-        <f>K28*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.559182623077112</v>
-      </c>
-      <c r="M28" s="41">
-        <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="O28" s="35">
-        <f t="shared" si="4"/>
-        <v>1.559182623077112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B29" s="73">
-        <f>MIN(B27:B28)</f>
-        <v>395.04400000000004</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" s="39">
-        <v>3.7</v>
-      </c>
-      <c r="F29" s="40">
-        <f>E29*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>126.63916380503954</v>
-      </c>
-      <c r="G29" s="41">
-        <f>$B$15/(F29*$B$44)</f>
-        <v>4.8134418662941096E-2</v>
-      </c>
-      <c r="H29" s="42">
-        <f t="shared" si="0"/>
-        <v>0.48134418662941092</v>
-      </c>
-      <c r="I29" s="42">
-        <f t="shared" si="5"/>
-        <v>0.96268837325882184</v>
-      </c>
-      <c r="J29" s="40">
-        <f>$B$21*F29*$B$14/($B$22*$B$40)</f>
-        <v>6226.4514808308859</v>
-      </c>
-      <c r="K29" s="43">
-        <f t="shared" si="2"/>
-        <v>3.5573527356037013E-2</v>
-      </c>
-      <c r="L29" s="41">
-        <f>K29*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5485391162274114</v>
-      </c>
-      <c r="M29" s="41">
-        <f t="shared" si="6"/>
-        <v>0.32432432432432429</v>
-      </c>
-      <c r="O29" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5485391162274114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E30" s="39">
-        <v>3.8</v>
+        <v>14.5</v>
       </c>
       <c r="F30" s="40">
         <f>E30*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>130.06184390787845</v>
+        <v>496.28861491164145</v>
       </c>
       <c r="G30" s="41">
         <f>$B$15/(F30*$B$44)</f>
-        <v>4.6867723434968957E-2</v>
+        <v>1.2282575796750485E-2</v>
       </c>
       <c r="H30" s="42">
         <f t="shared" si="0"/>
-        <v>0.46867723434968961</v>
+        <v>0.12282575796750486</v>
       </c>
       <c r="I30" s="42">
-        <f t="shared" si="5"/>
-        <v>0.93735446869937922</v>
+        <f t="shared" si="3"/>
+        <v>0.24565151593500972</v>
       </c>
       <c r="J30" s="40">
         <f>$B$21*F30*$B$14/($B$22*$B$40)</f>
-        <v>6394.733953285775</v>
+        <v>24400.958505958875</v>
       </c>
       <c r="K30" s="43">
         <f t="shared" si="2"/>
-        <v>3.5337145314187718E-2</v>
+        <v>2.5283393332657642E-2</v>
       </c>
       <c r="L30" s="41">
         <f>K30*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5382492499874467</v>
+        <v>1.1006027930468736</v>
       </c>
       <c r="M30" s="41">
-        <f t="shared" si="6"/>
-        <v>0.31578947368421051</v>
+        <f>100*(2*6/1000)/E30</f>
+        <v>8.2758620689655171E-2</v>
       </c>
       <c r="O30" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5382492499874467</v>
+        <f>IF($J30&lt;$B$17," ",$L30)</f>
+        <v>1.1006027930468736</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B31" s="74">
+        <f>MIN(B29:B30)</f>
+        <v>395.04400000000004</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>182</v>
+      </c>
       <c r="E31" s="39">
-        <v>3.9</v>
+        <v>15</v>
       </c>
       <c r="F31" s="40">
         <f>E31*$B$40^2/($B$23*$B$41*$B$42)</f>
-        <v>133.48452401071734</v>
+        <v>513.402015425836</v>
       </c>
       <c r="G31" s="41">
         <f>$B$15/(F31*$B$44)</f>
-        <v>4.5665986936636427E-2</v>
+        <v>1.187315660352547E-2</v>
       </c>
       <c r="H31" s="42">
         <f t="shared" si="0"/>
-        <v>0.45665986936636427</v>
+        <v>0.1187315660352547</v>
       </c>
       <c r="I31" s="42">
-        <f t="shared" si="5"/>
-        <v>0.91331973873272854</v>
+        <f t="shared" si="3"/>
+        <v>0.2374631320705094</v>
       </c>
       <c r="J31" s="40">
         <f>$B$21*F31*$B$14/($B$22*$B$40)</f>
-        <v>6563.0164257406623</v>
+        <v>25242.370868233324</v>
       </c>
       <c r="K31" s="43">
         <f t="shared" si="2"/>
-        <v>3.5108413909770438E-2</v>
+        <v>2.5070012287125413E-2</v>
       </c>
       <c r="L31" s="41">
         <f>K31*$B$15*$B$21*$B$43*$B$38/(2*$B$14*$B$45)</f>
-        <v>1.5282924210425748</v>
+        <v>1.0913141753520053</v>
       </c>
       <c r="M31" s="41">
-        <f t="shared" si="6"/>
-        <v>0.30769230769230771</v>
+        <f>100*(2*6/1000)/E31</f>
+        <v>0.08</v>
       </c>
       <c r="O31" s="35">
-        <f t="shared" si="4"/>
-        <v>1.5282924210425748</v>
+        <f>IF($J31&lt;$B$17," ",$L31)</f>
+        <v>1.0913141753520053</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -4191,6 +4222,17 @@
         <v>1000</v>
       </c>
       <c r="C45" s="35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="35">
+        <v>16.387063999999999</v>
+      </c>
+      <c r="C46" s="35" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4217,7 +4259,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4659,7 +4701,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4826,7 +4868,7 @@
       </c>
       <c r="B8" s="70">
         <f>Canisters!B11</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>62</v>
@@ -4848,7 +4890,7 @@
       </c>
       <c r="B9" s="9">
         <f>B8*B1+(24-B8)*B3</f>
-        <v>1338.1851697221482</v>
+        <v>1759.1908929628644</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>64</v>
@@ -4966,7 +5008,7 @@
       </c>
       <c r="B17" s="13">
         <f>(B9*B14*B16)/(B13*B15)</f>
-        <v>1773.0953498818465</v>
+        <v>2330.9279331757953</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>81</v>
@@ -4989,7 +5031,7 @@
       </c>
       <c r="F18" s="14">
         <f>IF(F14&lt;12, EVEN((B17/F15)*(B13/F14)), CEILING((B17/F15)*(B13/F14),1))</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
         <v>79</v>
@@ -5027,7 +5069,7 @@
       </c>
       <c r="B22" s="14">
         <f>$B$9/B21</f>
-        <v>334.54629243053705</v>
+        <v>439.7977232407161</v>
       </c>
       <c r="C22" t="s">
         <v>89</v>
@@ -5120,7 +5162,7 @@
       </c>
       <c r="B29" s="14">
         <f>$B$9/B28</f>
-        <v>669.0925848610741</v>
+        <v>879.59544648143219</v>
       </c>
       <c r="C29" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Create block diagram and detailed list of components for small PV array
Also includes preliminary list of additional components if we retain the
remote pump design.
</commit_message>
<xml_diff>
--- a/engr/calculations.xlsx
+++ b/engr/calculations.xlsx
@@ -864,7 +864,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="207">
   <si>
     <t>Running power</t>
   </si>
@@ -1146,12 +1146,6 @@
   </si>
   <si>
     <t>Solar array sizing (winter worst-case) [2]</t>
-  </si>
-  <si>
-    <t>Charge controller min. amperage</t>
-  </si>
-  <si>
-    <t>Amps in</t>
   </si>
   <si>
     <t>Wire size requirements [3]</t>
@@ -1545,6 +1539,18 @@
   </si>
   <si>
     <t>Rolls Surrette S-550</t>
+  </si>
+  <si>
+    <t>Charge controller rating</t>
+  </si>
+  <si>
+    <t>Safety factor</t>
+  </si>
+  <si>
+    <t>Worst case</t>
+  </si>
+  <si>
+    <t>Annual mean</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +1803,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1957,9 +1963,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1990,6 +1993,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3641,69 +3649,69 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B4" s="19">
         <v>1013</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B5" s="19">
         <v>923</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B6" s="19">
         <v>834</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B11" s="48">
         <v>55</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B12" s="49">
         <v>923</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3731,7 +3739,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25"/>
@@ -3770,34 +3778,34 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7" s="28">
         <v>6</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B8" s="28">
         <v>33</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" s="29">
         <v>0.1</v>
@@ -3805,46 +3813,46 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B10" s="28">
         <v>0.85</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="28">
         <v>24</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" s="30">
         <f>B7*(14.7/(B4/68.947573))*((B3+460)/530)</f>
         <v>6.4020229530019002</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" s="31">
         <f>ERF(B10/SQRT(2))</f>
@@ -3853,7 +3861,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B16" s="31">
         <f>(1-B15)/2</f>
@@ -3862,7 +3870,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" s="32">
         <f>B8*(0.528-B9)*1000/(B14*B16*60*B11)</f>
@@ -3910,60 +3918,60 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E1" s="34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="72"/>
+        <v>151</v>
+      </c>
+      <c r="H1" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="71"/>
       <c r="J1" s="33"/>
       <c r="K1" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L1" s="33"/>
       <c r="O1" s="33" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -3979,7 +3987,7 @@
         <f>Conditions!C11</f>
         <v>ºF</v>
       </c>
-      <c r="E3" s="68">
+      <c r="E3" s="67">
         <v>1</v>
       </c>
       <c r="F3" s="36">
@@ -4032,7 +4040,7 @@
         <f>Conditions!C12</f>
         <v>mbar</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="67">
         <v>1.5</v>
       </c>
       <c r="F4" s="36">
@@ -4073,7 +4081,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E5" s="68">
+      <c r="E5" s="67">
         <v>2</v>
       </c>
       <c r="F5" s="36">
@@ -4117,7 +4125,7 @@
       <c r="A6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="67">
         <v>2.5</v>
       </c>
       <c r="F6" s="36">
@@ -4159,15 +4167,15 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B7" s="33">
         <v>7</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="68">
+        <v>185</v>
+      </c>
+      <c r="E7" s="67">
         <v>3</v>
       </c>
       <c r="F7" s="36">
@@ -4209,12 +4217,12 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="68">
+        <v>139</v>
+      </c>
+      <c r="E8" s="67">
         <v>3.5</v>
       </c>
       <c r="F8" s="36">
@@ -4256,16 +4264,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B9" s="33">
         <f>0.25-2*0.047</f>
         <v>0.156</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" s="68">
+        <v>133</v>
+      </c>
+      <c r="E9" s="67">
         <v>4</v>
       </c>
       <c r="F9" s="36">
@@ -4307,16 +4315,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" s="33">
         <f>0.25-2*0.062</f>
         <v>0.126</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="68">
+        <v>133</v>
+      </c>
+      <c r="E10" s="67">
         <v>4.5</v>
       </c>
       <c r="F10" s="36">
@@ -4358,16 +4366,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B11" s="33">
         <f>0.125-2*0.047</f>
         <v>3.1E-2</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="68">
+        <v>133</v>
+      </c>
+      <c r="E11" s="67">
         <v>5</v>
       </c>
       <c r="F11" s="36">
@@ -4408,7 +4416,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E12" s="68">
+      <c r="E12" s="67">
         <v>5.5</v>
       </c>
       <c r="F12" s="36">
@@ -4450,9 +4458,9 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="E13" s="68">
+        <v>135</v>
+      </c>
+      <c r="E13" s="67">
         <v>6</v>
       </c>
       <c r="F13" s="36">
@@ -4494,15 +4502,15 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" s="68">
+        <v>134</v>
+      </c>
+      <c r="B14" s="67">
         <v>3.1E-2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="68">
+        <v>133</v>
+      </c>
+      <c r="E14" s="67">
         <v>6.5</v>
       </c>
       <c r="F14" s="36">
@@ -4544,15 +4552,15 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="68">
+        <v>132</v>
+      </c>
+      <c r="B15" s="67">
         <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="68">
+        <v>131</v>
+      </c>
+      <c r="E15" s="67">
         <v>7</v>
       </c>
       <c r="F15" s="36">
@@ -4594,15 +4602,15 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="B16" s="69">
+        <v>180</v>
+      </c>
+      <c r="B16" s="68">
         <v>50</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="E16" s="68">
+        <v>168</v>
+      </c>
+      <c r="E16" s="67">
         <v>7.5</v>
       </c>
       <c r="F16" s="36">
@@ -4644,12 +4652,12 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="69">
+        <v>183</v>
+      </c>
+      <c r="B17" s="68">
         <v>4100</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="67">
         <v>8</v>
       </c>
       <c r="F17" s="36">
@@ -4690,7 +4698,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E18" s="68">
+      <c r="E18" s="67">
         <v>8.5</v>
       </c>
       <c r="F18" s="36">
@@ -4732,9 +4740,9 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="68">
+        <v>112</v>
+      </c>
+      <c r="E19" s="67">
         <v>9</v>
       </c>
       <c r="F19" s="36">
@@ -4776,16 +4784,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B20" s="42">
         <f>(B3-32)*5/9</f>
         <v>12.777777777777779</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="68">
+        <v>110</v>
+      </c>
+      <c r="E20" s="67">
         <v>9.5</v>
       </c>
       <c r="F20" s="36">
@@ -4827,16 +4835,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" s="43">
         <f>1000*(B4/B38)/(B34*(B20+273.15))</f>
         <v>1.1245420441113285</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="68">
+        <v>108</v>
+      </c>
+      <c r="E21" s="67">
         <v>10</v>
       </c>
       <c r="F21" s="36">
@@ -4878,16 +4886,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B22" s="44">
         <f>B36*(B20+273.15)^1.5/((B20+273.15+B35)*10^6)</f>
         <v>1.8009406563349156E-5</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="68">
+        <v>106</v>
+      </c>
+      <c r="E22" s="67">
         <v>10.5</v>
       </c>
       <c r="F22" s="36">
@@ -4929,16 +4937,16 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" s="45">
         <f>PI()*(B14/2)^2</f>
         <v>7.5476763502494771E-4</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="68">
+        <v>104</v>
+      </c>
+      <c r="E23" s="67">
         <v>11</v>
       </c>
       <c r="F23" s="36">
@@ -4980,16 +4988,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B24" s="67">
+        <v>190</v>
+      </c>
+      <c r="B24" s="66">
         <f>$B$15*$B$23*$B$43*$B$46</f>
         <v>2.9684221296677897</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="68">
+        <v>191</v>
+      </c>
+      <c r="E24" s="67">
         <v>11.5</v>
       </c>
       <c r="F24" s="36">
@@ -5031,13 +5039,13 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="71">
+        <v>193</v>
+      </c>
+      <c r="B25" s="70">
         <f>(B24/B42)/(Canisters!B8*(0.528-Canisters!B9))</f>
         <v>2.1016865828857187E-4</v>
       </c>
-      <c r="E25" s="68">
+      <c r="E25" s="67">
         <v>12</v>
       </c>
       <c r="F25" s="36">
@@ -5079,16 +5087,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26" s="47">
         <f>-1*B7*B39</f>
         <v>-482.58</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="E26" s="68">
+        <v>186</v>
+      </c>
+      <c r="E26" s="67">
         <v>12.5</v>
       </c>
       <c r="F26" s="36">
@@ -5130,16 +5138,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B27" s="47">
         <f>-1*(1-$B$37)*$B$4-$B$16</f>
         <v>-485.65599999999995</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="E27" s="68">
+        <v>186</v>
+      </c>
+      <c r="E27" s="67">
         <v>13</v>
       </c>
       <c r="F27" s="36">
@@ -5181,16 +5189,16 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B28" s="47">
         <f>$B$4*$B$37</f>
         <v>487.34400000000005</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="E28" s="68">
+        <v>177</v>
+      </c>
+      <c r="E28" s="67">
         <v>13.5</v>
       </c>
       <c r="F28" s="36">
@@ -5232,16 +5240,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B29" s="47">
         <f>$B$4+MIN($B$26:$B$27)-MAX($O$3:$O$31)</f>
         <v>435.63600101214121</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="E29" s="68">
+        <v>177</v>
+      </c>
+      <c r="E29" s="67">
         <v>14</v>
       </c>
       <c r="F29" s="36">
@@ -5283,16 +5291,16 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B30" s="47">
         <f>$B$4*($B$37-Canisters!B9)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="E30" s="68">
+        <v>177</v>
+      </c>
+      <c r="E30" s="67">
         <v>14.5</v>
       </c>
       <c r="F30" s="36">
@@ -5334,16 +5342,16 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B31" s="70">
+        <v>189</v>
+      </c>
+      <c r="B31" s="69">
         <f>MIN(B29:B30)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="E31" s="68">
+        <v>177</v>
+      </c>
+      <c r="E31" s="67">
         <v>15</v>
       </c>
       <c r="F31" s="36">
@@ -5385,45 +5393,45 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" s="41">
         <v>287.05799999999999</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" s="33">
         <v>120</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B36" s="33">
         <v>1.512041288</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B37" s="33">
         <v>0.52800000000000002</v>
@@ -5431,101 +5439,101 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B38" s="33">
         <v>10</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B39" s="33">
         <v>68.94</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B40" s="33">
         <v>39.369999999999997</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41" s="33">
         <v>60</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" s="33">
         <v>1000</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B43" s="33">
         <v>12</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B44" s="33">
         <v>3.2810000000000001</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45" s="33">
         <v>1000</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B46" s="33">
         <v>16.387063999999999</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5551,7 +5559,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5574,7 +5582,7 @@
       </c>
       <c r="I1" s="14">
         <f>SUM(I5:I30)</f>
-        <v>20.499620540119341</v>
+        <v>73.299620540119349</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -5615,7 +5623,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>10</v>
@@ -5631,13 +5639,13 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="74">
         <v>1</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="74">
         <v>12</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="75">
         <v>0.01</v>
       </c>
       <c r="G5" s="1">
@@ -5665,13 +5673,13 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="74">
         <v>1</v>
       </c>
-      <c r="E6" s="75">
+      <c r="E6" s="74">
         <v>12</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="75">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G6" s="1">
@@ -5696,13 +5704,13 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="74">
         <v>1</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="74">
         <v>12</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="75">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G7" s="1">
@@ -5727,13 +5735,13 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="74">
         <v>2</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="74">
         <v>12</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="75">
         <v>0.01</v>
       </c>
       <c r="G8" s="1">
@@ -5758,13 +5766,13 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="74">
         <v>1</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="74">
         <v>12</v>
       </c>
-      <c r="F9" s="76">
+      <c r="F9" s="75">
         <v>0.01</v>
       </c>
       <c r="G9" s="1">
@@ -5789,13 +5797,13 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="74">
         <v>1</v>
       </c>
-      <c r="E10" s="75">
+      <c r="E10" s="74">
         <v>12</v>
       </c>
-      <c r="F10" s="76">
+      <c r="F10" s="75">
         <v>0.11</v>
       </c>
       <c r="G10" s="1">
@@ -5820,13 +5828,13 @@
       <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="75">
+      <c r="D11" s="74">
         <v>1</v>
       </c>
-      <c r="E11" s="75">
+      <c r="E11" s="74">
         <v>12</v>
       </c>
-      <c r="F11" s="76">
+      <c r="F11" s="75">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G11" s="1">
@@ -5842,9 +5850,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="76"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="75"/>
       <c r="G12" s="1">
         <f t="shared" ref="G12" si="2">E12*F12</f>
         <v>0</v>
@@ -5867,13 +5875,13 @@
       <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="75">
+      <c r="D13" s="74">
         <v>2</v>
       </c>
-      <c r="E13" s="75">
+      <c r="E13" s="74">
         <v>12</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="75">
         <v>1</v>
       </c>
       <c r="G13" s="1">
@@ -5900,15 +5908,15 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="75">
+        <v>197</v>
+      </c>
+      <c r="D14" s="74">
         <v>2</v>
       </c>
-      <c r="E14" s="75">
+      <c r="E14" s="74">
         <v>5</v>
       </c>
-      <c r="F14" s="76">
+      <c r="F14" s="75">
         <v>1.2E-2</v>
       </c>
       <c r="G14" s="1">
@@ -5934,13 +5942,13 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="75">
+      <c r="D15" s="74">
         <v>1</v>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="74">
         <v>12</v>
       </c>
-      <c r="F15" s="76">
+      <c r="F15" s="75">
         <v>0.25</v>
       </c>
       <c r="G15" s="1">
@@ -5960,18 +5968,18 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="75">
-        <v>0</v>
-      </c>
-      <c r="E16" s="75">
+      <c r="D16" s="74">
+        <v>1</v>
+      </c>
+      <c r="E16" s="74">
         <v>12</v>
       </c>
-      <c r="F16" s="76">
+      <c r="F16" s="75">
         <v>5.2</v>
       </c>
       <c r="G16" s="1">
@@ -5983,7 +5991,7 @@
       </c>
       <c r="I16" s="50">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>62.400000000000006</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -5991,18 +5999,18 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="75">
-        <v>2</v>
-      </c>
-      <c r="E17" s="75">
+        <v>195</v>
+      </c>
+      <c r="D17" s="74">
+        <v>0</v>
+      </c>
+      <c r="E17" s="74">
         <v>12</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="75">
         <v>0.4</v>
       </c>
       <c r="G17" s="1">
@@ -6014,7 +6022,7 @@
       </c>
       <c r="I17" s="50">
         <f t="shared" si="1"/>
-        <v>9.6000000000000014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -6022,18 +6030,18 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
-      </c>
-      <c r="D18" s="75">
+        <v>199</v>
+      </c>
+      <c r="D18" s="74">
         <v>0</v>
       </c>
-      <c r="E18" s="75">
+      <c r="E18" s="74">
         <v>12</v>
       </c>
-      <c r="F18" s="76">
+      <c r="F18" s="75">
         <f>130/E18</f>
         <v>10.833333333333334</v>
       </c>
@@ -6068,7 +6076,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6093,16 +6101,16 @@
       </c>
       <c r="B1" s="16">
         <f>Consumption!I1</f>
-        <v>20.499620540119341</v>
+        <v>73.299620540119349</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
       <c r="I1" s="4" t="s">
         <v>46</v>
       </c>
@@ -6110,7 +6118,7 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="16">
         <f>B1/B13</f>
-        <v>1.7083017116766117</v>
+        <v>6.1083017116766127</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -6122,10 +6130,10 @@
         <v>47</v>
       </c>
       <c r="G2" s="53"/>
-      <c r="J2" s="73" t="s">
+      <c r="J2" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="73"/>
+      <c r="K2" s="72"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -6233,7 +6241,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="66">
+      <c r="B8" s="65">
         <f>Canisters!B11</f>
         <v>24</v>
       </c>
@@ -6257,7 +6265,7 @@
       </c>
       <c r="B9" s="9">
         <f>B8*B1+(24-B8)*B3</f>
-        <v>491.99089296286422</v>
+        <v>1759.1908929628644</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>62</v>
@@ -6305,17 +6313,17 @@
       <c r="E13" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="74" t="s">
-        <v>204</v>
-      </c>
-      <c r="G13" s="74"/>
+      <c r="F13" s="73" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="73"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="11">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>69</v>
@@ -6336,16 +6344,16 @@
         <v>71</v>
       </c>
       <c r="B15" s="12">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="79">
+      <c r="F15" s="78">
         <f>-116.5*LN(B2)+771.1</f>
-        <v>708.7142819271786</v>
+        <v>560.27591686377491</v>
       </c>
       <c r="G15" t="s">
         <v>73</v>
@@ -6376,7 +6384,7 @@
       </c>
       <c r="B17" s="13">
         <f>(B9*B14*B16)/(B13*B15)</f>
-        <v>1043.0206930812719</v>
+        <v>1864.7423465406364</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>78</v>
@@ -6387,7 +6395,7 @@
       </c>
       <c r="F17" s="14">
         <f>F15*F16*(F14/B13)</f>
-        <v>1417.4285638543572</v>
+        <v>1120.5518337275498</v>
       </c>
       <c r="G17" t="s">
         <v>73</v>
@@ -6399,7 +6407,7 @@
       </c>
       <c r="F18" s="14">
         <f>IF(F14&lt;12, EVEN((B17/F15)*(B13/F14)), CEILING((B17/F15)*(B13/F14),1))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
         <v>76</v>
@@ -6426,10 +6434,10 @@
       <c r="E21" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="74"/>
+      <c r="G21" s="73"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -6437,7 +6445,7 @@
       </c>
       <c r="B22" s="14">
         <f>$B$9/B21</f>
-        <v>122.99772324071606</v>
+        <v>439.7977232407161</v>
       </c>
       <c r="C22" t="s">
         <v>86</v>
@@ -6458,7 +6466,7 @@
       </c>
       <c r="B23" s="1">
         <f>CEILING(B22/F24,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>89</v>
@@ -6479,7 +6487,7 @@
       </c>
       <c r="B24" s="14">
         <f>B23*F22</f>
-        <v>8.3000000000000007</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -6500,7 +6508,7 @@
         <v>93</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>94</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -6513,15 +6521,11 @@
       <c r="C28" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="14">
-        <f>B31/G28</f>
-        <v>10.375</v>
-      </c>
-      <c r="F28" t="s">
-        <v>95</v>
-      </c>
-      <c r="G28" s="65">
-        <v>0.8</v>
+      <c r="E28" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="81">
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -6530,13 +6534,21 @@
       </c>
       <c r="B29" s="14">
         <f>$B$9/B28</f>
-        <v>245.99544648143211</v>
+        <v>879.59544648143219</v>
       </c>
       <c r="C29" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="14"/>
-      <c r="G29" s="1"/>
+      <c r="E29" s="80" t="s">
+        <v>206</v>
+      </c>
+      <c r="F29" s="14">
+        <f>B24/(1-F28)</f>
+        <v>20.75</v>
+      </c>
+      <c r="G29" s="79" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -6544,10 +6556,20 @@
       </c>
       <c r="B30" s="1">
         <f>CEILING(B29/F24,1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>89</v>
+      </c>
+      <c r="E30" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="F30" s="14">
+        <f>B31/(1-F28)</f>
+        <v>31.125</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -6556,7 +6578,7 @@
       </c>
       <c r="B31" s="14">
         <f>B30*F22</f>
-        <v>8.3000000000000007</v>
+        <v>24.900000000000002</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -6564,12 +6586,12 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1">
         <f>F23</f>
@@ -6581,32 +6603,32 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -6648,138 +6670,138 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="77" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="77"/>
+    <col min="1" max="1" width="11.28515625" style="76" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="76"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="77" t="s">
+      <c r="A1" s="76" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="78" t="s">
-        <v>202</v>
+      <c r="D1" s="77" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="77">
+      <c r="A2" s="76">
         <v>554</v>
       </c>
-      <c r="B2" s="77">
+      <c r="B2" s="76">
         <v>5.54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="77">
+      <c r="A3" s="76">
         <v>524</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="76">
         <v>7.28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="77">
+      <c r="A4" s="76">
         <v>500</v>
       </c>
-      <c r="B4" s="77">
+      <c r="B4" s="76">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="77">
+      <c r="A5" s="76">
         <v>441</v>
       </c>
-      <c r="B5" s="77">
+      <c r="B5" s="76">
         <v>18.37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="77">
+      <c r="A6" s="76">
         <v>428</v>
       </c>
-      <c r="B6" s="77">
+      <c r="B6" s="76">
         <v>21.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="77">
+      <c r="A7" s="76">
         <v>401</v>
       </c>
-      <c r="B7" s="77">
+      <c r="B7" s="76">
         <v>26.76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="77">
+      <c r="A8" s="76">
         <v>381</v>
       </c>
-      <c r="B8" s="77">
+      <c r="B8" s="76">
         <v>31.74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="77">
+      <c r="A9" s="76">
         <v>364</v>
       </c>
-      <c r="B9" s="77">
+      <c r="B9" s="76">
         <v>36.380000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="77">
+      <c r="A10" s="76">
         <v>342</v>
       </c>
-      <c r="B10" s="77">
+      <c r="B10" s="76">
         <v>42.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="77">
+      <c r="A11" s="76">
         <v>317</v>
       </c>
-      <c r="B11" s="77">
+      <c r="B11" s="76">
         <v>52.79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="77">
+      <c r="A12" s="76">
         <v>300</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="76">
         <v>59.92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="77">
+      <c r="A13" s="76">
         <v>278</v>
       </c>
-      <c r="B13" s="77">
+      <c r="B13" s="76">
         <v>69.55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+      <c r="A14" s="76">
         <v>253</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="76">
         <v>84.17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="77">
+      <c r="A15" s="76">
         <v>218</v>
       </c>
-      <c r="B15" s="77">
+      <c r="B15" s="76">
         <v>109.14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="77">
+      <c r="A16" s="76">
         <v>154</v>
       </c>
-      <c r="B16" s="77">
+      <c r="B16" s="76">
         <v>154.08000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revise calcs with slightly smaller solar panel
Low power consumption design was approved. Select solar panel with
slightly smaller power output and physical dimensions to better match
power consumption and to fit better on a smaller trailer (4x6 not 5x8).
</commit_message>
<xml_diff>
--- a/engr/calculations.xlsx
+++ b/engr/calculations.xlsx
@@ -864,7 +864,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="206">
   <si>
     <t>Running power</t>
   </si>
@@ -987,9 +987,6 @@
   </si>
   <si>
     <t>Pump</t>
-  </si>
-  <si>
-    <t>12Vdc @ 5.2A</t>
   </si>
   <si>
     <t>Valve control relay</t>
@@ -1520,18 +1517,9 @@
     <t>9-14Vdc @ 0.4A</t>
   </si>
   <si>
-    <t>NPK09 (KNF)</t>
-  </si>
-  <si>
     <t>12mA @ logic voltage (1mA off-state leakage)</t>
   </si>
   <si>
-    <t>NPK 018 DC vacuum(KNF)</t>
-  </si>
-  <si>
-    <t>130W (AC model, DC specs not given)</t>
-  </si>
-  <si>
     <t>Rolls S-550 deep cycle battery</t>
   </si>
   <si>
@@ -1551,6 +1539,15 @@
   </si>
   <si>
     <t>Annual mean</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>CHSM6610P-255</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1800,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1975,15 +1972,6 @@
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1998,6 +1986,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2158,7 +2158,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2392,11 +2391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="254846688"/>
-        <c:axId val="254849432"/>
+        <c:axId val="236351632"/>
+        <c:axId val="236838112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254846688"/>
+        <c:axId val="236351632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2450,7 +2449,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2517,12 +2515,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254849432"/>
+        <c:crossAx val="236838112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254849432"/>
+        <c:axId val="236838112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2568,7 +2566,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2635,7 +2632,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254846688"/>
+        <c:crossAx val="236351632"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3642,76 +3639,76 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4" s="19">
         <v>1013</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="19">
         <v>923</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="19">
         <v>834</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="48">
         <v>55</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="49">
         <v>923</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3739,7 +3736,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25"/>
@@ -3778,34 +3775,34 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="28">
         <v>6</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" s="28">
         <v>33</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="29">
         <v>0.1</v>
@@ -3813,46 +3810,46 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" s="28">
         <v>0.85</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="28">
         <v>24</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" s="30">
         <f>B7*(14.7/(B4/68.947573))*((B3+460)/530)</f>
         <v>6.4020229530019002</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15" s="31">
         <f>ERF(B10/SQRT(2))</f>
@@ -3861,7 +3858,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B16" s="31">
         <f>(1-B15)/2</f>
@@ -3870,14 +3867,14 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B17" s="32">
         <f>B8*(0.528-B9)*1000/(B14*B16*60*B11)</f>
         <v>7.7509263683374092</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3894,7 +3891,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3918,60 +3915,60 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E1" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="71"/>
+      <c r="H1" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="79"/>
       <c r="J1" s="33"/>
       <c r="K1" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L1" s="33"/>
       <c r="O1" s="33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M2" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="O2" s="34" t="s">
         <v>142</v>
-      </c>
-      <c r="O2" s="34" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -4123,7 +4120,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="67">
         <v>2.5</v>
@@ -4167,13 +4164,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="33">
         <v>7</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="67">
         <v>3</v>
@@ -4217,10 +4214,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="67">
         <v>3.5</v>
@@ -4264,14 +4261,14 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" s="33">
         <f>0.25-2*0.047</f>
         <v>0.156</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" s="67">
         <v>4</v>
@@ -4315,14 +4312,14 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="33">
         <f>0.25-2*0.062</f>
         <v>0.126</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E10" s="67">
         <v>4.5</v>
@@ -4366,14 +4363,14 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="33">
         <f>0.125-2*0.047</f>
         <v>3.1E-2</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="67">
         <v>5</v>
@@ -4458,7 +4455,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="67">
         <v>6</v>
@@ -4502,13 +4499,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="67">
         <v>3.1E-2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="67">
         <v>6.5</v>
@@ -4552,13 +4549,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" s="67">
         <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" s="67">
         <v>7</v>
@@ -4602,13 +4599,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B16" s="68">
         <v>50</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E16" s="67">
         <v>7.5</v>
@@ -4652,7 +4649,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="68">
         <v>4100</v>
@@ -4740,7 +4737,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="67">
         <v>9</v>
@@ -4784,14 +4781,14 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="42">
         <f>(B3-32)*5/9</f>
         <v>12.777777777777779</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" s="67">
         <v>9.5</v>
@@ -4835,14 +4832,14 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" s="43">
         <f>1000*(B4/B38)/(B34*(B20+273.15))</f>
         <v>1.1245420441113285</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" s="67">
         <v>10</v>
@@ -4886,14 +4883,14 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="44">
         <f>B36*(B20+273.15)^1.5/((B20+273.15+B35)*10^6)</f>
         <v>1.8009406563349156E-5</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="67">
         <v>10.5</v>
@@ -4937,14 +4934,14 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="45">
         <f>PI()*(B14/2)^2</f>
         <v>7.5476763502494771E-4</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="67">
         <v>11</v>
@@ -4988,14 +4985,14 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" s="66">
         <f>$B$15*$B$23*$B$43*$B$46</f>
         <v>2.9684221296677897</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E24" s="67">
         <v>11.5</v>
@@ -5039,7 +5036,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B25" s="70">
         <f>(B24/B42)/(Canisters!B8*(0.528-Canisters!B9))</f>
@@ -5087,14 +5084,14 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="47">
         <f>-1*B7*B39</f>
         <v>-482.58</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E26" s="67">
         <v>12.5</v>
@@ -5138,14 +5135,14 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B27" s="47">
         <f>-1*(1-$B$37)*$B$4-$B$16</f>
         <v>-485.65599999999995</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E27" s="67">
         <v>13</v>
@@ -5189,14 +5186,14 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="47">
         <f>$B$4*$B$37</f>
         <v>487.34400000000005</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E28" s="67">
         <v>13.5</v>
@@ -5240,14 +5237,14 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B29" s="47">
         <f>$B$4+MIN($B$26:$B$27)-MAX($O$3:$O$31)</f>
         <v>435.63600101214121</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29" s="67">
         <v>14</v>
@@ -5291,14 +5288,14 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B30" s="47">
         <f>$B$4*($B$37-Canisters!B9)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E30" s="67">
         <v>14.5</v>
@@ -5342,14 +5339,14 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="69">
         <f>MIN(B29:B30)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E31" s="67">
         <v>15</v>
@@ -5393,45 +5390,45 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" s="41">
         <v>287.05799999999999</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="33">
         <v>120</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="33">
         <v>1.512041288</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" s="33">
         <v>0.52800000000000002</v>
@@ -5439,101 +5436,101 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B38" s="33">
         <v>10</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="33">
         <v>68.94</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" s="33">
         <v>39.369999999999997</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" s="33">
         <v>60</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" s="33">
         <v>1000</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" s="33">
         <v>12</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="33">
         <v>3.2810000000000001</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="33">
         <v>1000</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B46" s="33">
         <v>16.387063999999999</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -5556,7 +5553,7 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -5581,8 +5578,8 @@
         <v>0</v>
       </c>
       <c r="I1" s="14">
-        <f>SUM(I5:I30)</f>
-        <v>73.299620540119349</v>
+        <f>SUM(I5:I28)</f>
+        <v>20.499620540119341</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -5623,7 +5620,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>10</v>
@@ -5639,13 +5636,13 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="71">
         <v>1</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="71">
         <v>12</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="72">
         <v>0.01</v>
       </c>
       <c r="G5" s="1">
@@ -5673,13 +5670,13 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="71">
         <v>1</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="71">
         <v>12</v>
       </c>
-      <c r="F6" s="75">
+      <c r="F6" s="72">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G6" s="1">
@@ -5690,7 +5687,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="50">
-        <f t="shared" ref="I6:I17" si="1">G6*D6*H6</f>
+        <f t="shared" ref="I6:I16" si="1">G6*D6*H6</f>
         <v>0.51600000000000001</v>
       </c>
     </row>
@@ -5704,13 +5701,13 @@
       <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="71">
         <v>1</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E7" s="71">
         <v>12</v>
       </c>
-      <c r="F7" s="75">
+      <c r="F7" s="72">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G7" s="1">
@@ -5735,13 +5732,13 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="71">
         <v>2</v>
       </c>
-      <c r="E8" s="74">
+      <c r="E8" s="71">
         <v>12</v>
       </c>
-      <c r="F8" s="75">
+      <c r="F8" s="72">
         <v>0.01</v>
       </c>
       <c r="G8" s="1">
@@ -5766,13 +5763,13 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="74">
+      <c r="D9" s="71">
         <v>1</v>
       </c>
-      <c r="E9" s="74">
+      <c r="E9" s="71">
         <v>12</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="72">
         <v>0.01</v>
       </c>
       <c r="G9" s="1">
@@ -5797,13 +5794,13 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="74">
+      <c r="D10" s="71">
         <v>1</v>
       </c>
-      <c r="E10" s="74">
+      <c r="E10" s="71">
         <v>12</v>
       </c>
-      <c r="F10" s="75">
+      <c r="F10" s="72">
         <v>0.11</v>
       </c>
       <c r="G10" s="1">
@@ -5828,13 +5825,13 @@
       <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="74">
+      <c r="D11" s="71">
         <v>1</v>
       </c>
-      <c r="E11" s="74">
+      <c r="E11" s="71">
         <v>12</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="72">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G11" s="1">
@@ -5850,9 +5847,9 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="75"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="1">
         <f t="shared" ref="G12" si="2">E12*F12</f>
         <v>0</v>
@@ -5875,13 +5872,13 @@
       <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="74">
+      <c r="D13" s="71">
         <v>2</v>
       </c>
-      <c r="E13" s="74">
+      <c r="E13" s="71">
         <v>12</v>
       </c>
-      <c r="F13" s="75">
+      <c r="F13" s="72">
         <v>1</v>
       </c>
       <c r="G13" s="1">
@@ -5902,21 +5899,21 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
       <c r="C14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D14" s="74">
+        <v>195</v>
+      </c>
+      <c r="D14" s="71">
         <v>2</v>
       </c>
-      <c r="E14" s="74">
+      <c r="E14" s="71">
         <v>5</v>
       </c>
-      <c r="F14" s="75">
+      <c r="F14" s="72">
         <v>1.2E-2</v>
       </c>
       <c r="G14" s="1">
@@ -5942,13 +5939,13 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="74">
+      <c r="D15" s="71">
         <v>1</v>
       </c>
-      <c r="E15" s="74">
+      <c r="E15" s="71">
         <v>12</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="72">
         <v>0.25</v>
       </c>
       <c r="G15" s="1">
@@ -5968,93 +5965,30 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="74">
-        <v>1</v>
-      </c>
-      <c r="E16" s="74">
+        <v>194</v>
+      </c>
+      <c r="D16" s="71">
+        <v>2</v>
+      </c>
+      <c r="E16" s="71">
         <v>12</v>
       </c>
-      <c r="F16" s="75">
-        <v>5.2</v>
+      <c r="F16" s="72">
+        <v>0.4</v>
       </c>
       <c r="G16" s="1">
         <f>E16*F16</f>
-        <v>62.400000000000006</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="H16" s="15">
         <v>1</v>
       </c>
       <c r="I16" s="50">
         <f t="shared" si="1"/>
-        <v>62.400000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D17" s="74">
-        <v>0</v>
-      </c>
-      <c r="E17" s="74">
-        <v>12</v>
-      </c>
-      <c r="F17" s="75">
-        <v>0.4</v>
-      </c>
-      <c r="G17" s="1">
-        <f>E17*F17</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="H17" s="15">
-        <v>1</v>
-      </c>
-      <c r="I17" s="50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" t="s">
-        <v>199</v>
-      </c>
-      <c r="D18" s="74">
-        <v>0</v>
-      </c>
-      <c r="E18" s="74">
-        <v>12</v>
-      </c>
-      <c r="F18" s="75">
-        <f>130/E18</f>
-        <v>10.833333333333334</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" ref="G18" si="4">E18*F18</f>
-        <v>130</v>
-      </c>
-      <c r="H18" s="15">
-        <v>1</v>
-      </c>
-      <c r="I18" s="50">
-        <f t="shared" ref="I18" si="5">G18*D18*H18</f>
-        <v>0</v>
+        <v>9.6000000000000014</v>
       </c>
     </row>
   </sheetData>
@@ -6076,7 +6010,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F22" sqref="F22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6097,47 +6031,47 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="16">
         <f>Consumption!I1</f>
-        <v>73.299620540119349</v>
+        <v>20.499620540119341</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="I1" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="I1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="16">
         <f>B1/B13</f>
-        <v>6.1083017116766127</v>
+        <v>1.7083017116766117</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="53"/>
+      <c r="J2" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="53"/>
-      <c r="J2" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="72"/>
+      <c r="K2" s="80"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="16">
         <f>Consumption!I2</f>
@@ -6147,22 +6081,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="G3" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="I3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -6183,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="1">
         <v>4</v>
@@ -6192,7 +6126,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -6223,7 +6157,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="60">
         <v>50</v>
@@ -6239,14 +6173,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="65">
         <f>Canisters!B11</f>
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="60">
@@ -6261,14 +6195,14 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="9">
         <f>B8*B1+(24-B8)*B3</f>
-        <v>1759.1908929628644</v>
+        <v>491.99089296286422</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="60">
         <v>30</v>
@@ -6293,44 +6227,44 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="10">
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="73" t="s">
-        <v>202</v>
-      </c>
-      <c r="G13" s="73"/>
+        <v>66</v>
+      </c>
+      <c r="F13" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="G13" s="81"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="11">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="B14" s="11">
-        <v>4</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="7">
         <v>6</v>
@@ -6341,7 +6275,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="12">
         <v>0.5</v>
@@ -6349,19 +6283,19 @@
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="75">
+        <f>-116.5*LN(B2)+771.1</f>
+        <v>708.7142819271786</v>
+      </c>
+      <c r="G15" t="s">
         <v>72</v>
-      </c>
-      <c r="F15" s="78">
-        <f>-116.5*LN(B2)+771.1</f>
-        <v>560.27591686377491</v>
-      </c>
-      <c r="G15" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" s="11">
         <v>1.59</v>
@@ -6369,216 +6303,225 @@
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="13">
         <f>(B9*B14*B16)/(B13*B15)</f>
-        <v>1864.7423465406364</v>
+        <v>1303.7758663515901</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F17" s="14">
         <f>F15*F16*(F14/B13)</f>
-        <v>1120.5518337275498</v>
+        <v>1417.4285638543572</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="14">
         <f>IF(F14&lt;12, EVEN((B17/F15)*(B13/F14)), CEILING((B17/F15)*(B13/F14),1))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="11">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="73" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="73"/>
+        <v>203</v>
+      </c>
+      <c r="F21" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="82"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="14">
         <f>$B$9/B21</f>
-        <v>439.7977232407161</v>
+        <v>122.99772324071606</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="7">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" s="81"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="1">
+        <f>CEILING(B22/F25,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="1">
-        <f>CEILING(B22/F24,1)</f>
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F23" s="7">
-        <v>35.72</v>
+        <v>8.33</v>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="14">
-        <f>B23*F22</f>
-        <v>16.600000000000001</v>
+        <f>B23*F23</f>
+        <v>8.33</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="7">
+        <v>30.68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="1">
+        <f>ROUND(F24*F23, 0)</f>
+        <v>256</v>
+      </c>
+      <c r="G25" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="1">
-        <f>ROUND(F23*F22, 0)</f>
-        <v>296</v>
-      </c>
-      <c r="G24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="11">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="79" t="s">
-        <v>204</v>
-      </c>
-      <c r="F28" s="81">
+        <v>59</v>
+      </c>
+      <c r="E28" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" s="78">
         <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="14">
         <f>$B$9/B28</f>
-        <v>879.59544648143219</v>
+        <v>245.99544648143211</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="80" t="s">
-        <v>206</v>
+        <v>85</v>
+      </c>
+      <c r="E29" s="77" t="s">
+        <v>202</v>
       </c>
       <c r="F29" s="14">
         <f>B24/(1-F28)</f>
-        <v>20.75</v>
-      </c>
-      <c r="G29" s="79" t="s">
+        <v>10.4125</v>
+      </c>
+      <c r="G29" s="76" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="1">
+        <f>CEILING(B29/F25,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="1">
-        <f>CEILING(B29/F24,1)</f>
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="79" t="s">
-        <v>205</v>
+      <c r="E30" s="76" t="s">
+        <v>201</v>
       </c>
       <c r="F30" s="14">
         <f>B31/(1-F28)</f>
-        <v>31.125</v>
-      </c>
-      <c r="G30" s="79" t="s">
+        <v>10.4125</v>
+      </c>
+      <c r="G30" s="76" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="14">
-        <f>B30*F22</f>
-        <v>24.900000000000002</v>
+        <f>B30*F23</f>
+        <v>8.33</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -6586,16 +6529,16 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="1">
-        <f>F23</f>
-        <v>35.72</v>
+        <f>F24</f>
+        <v>30.68</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -6603,39 +6546,40 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="F21:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="F17">
@@ -6670,138 +6614,138 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="76" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="76"/>
+    <col min="1" max="1" width="11.28515625" style="73" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="76" t="s">
+      <c r="A1" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="77" t="s">
-        <v>200</v>
+      <c r="D1" s="74" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="76">
+      <c r="A2" s="73">
         <v>554</v>
       </c>
-      <c r="B2" s="76">
+      <c r="B2" s="73">
         <v>5.54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="76">
+      <c r="A3" s="73">
         <v>524</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="73">
         <v>7.28</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="76">
+      <c r="A4" s="73">
         <v>500</v>
       </c>
-      <c r="B4" s="76">
+      <c r="B4" s="73">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="76">
+      <c r="A5" s="73">
         <v>441</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="73">
         <v>18.37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="76">
+      <c r="A6" s="73">
         <v>428</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="73">
         <v>21.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="76">
+      <c r="A7" s="73">
         <v>401</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="73">
         <v>26.76</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="76">
+      <c r="A8" s="73">
         <v>381</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="73">
         <v>31.74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="76">
+      <c r="A9" s="73">
         <v>364</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="73">
         <v>36.380000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="76">
+      <c r="A10" s="73">
         <v>342</v>
       </c>
-      <c r="B10" s="76">
+      <c r="B10" s="73">
         <v>42.8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="76">
+      <c r="A11" s="73">
         <v>317</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="73">
         <v>52.79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="76">
+      <c r="A12" s="73">
         <v>300</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="73">
         <v>59.92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="76">
+      <c r="A13" s="73">
         <v>278</v>
       </c>
-      <c r="B13" s="76">
+      <c r="B13" s="73">
         <v>69.55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="76">
+      <c r="A14" s="73">
         <v>253</v>
       </c>
-      <c r="B14" s="76">
+      <c r="B14" s="73">
         <v>84.17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="76">
+      <c r="A15" s="73">
         <v>218</v>
       </c>
-      <c r="B15" s="76">
+      <c r="B15" s="73">
         <v>109.14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="76">
+      <c r="A16" s="73">
         <v>154</v>
       </c>
-      <c r="B16" s="76">
+      <c r="B16" s="73">
         <v>154.08000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIX: Revise calcs using actual power generated & decrease solar panel size
Since charge controller is pulse-width modulation, actual power produced
is determined by battery voltage and available current through PV array.
Update calculations to use the actual instead of rated power when
evaluating req'd number of solar panels.

Also check to ensure solar panel output voltage falls within ratings of
charge controller.

And since low power consumption design was approved, select solar panel
with smaller power output and physical dimensions to better match
power consumption and to fit better on a smaller trailer (4x6 not 5x8).
</commit_message>
<xml_diff>
--- a/engr/calculations.xlsx
+++ b/engr/calculations.xlsx
@@ -859,12 +859,132 @@
         </r>
       </text>
     </comment>
+    <comment ref="E23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum power voltage. Recommended &gt; battery regulation voltage by 5%+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maximum power current. Cannot exceed charge controller rating</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Open circuit voltage. Must not exceed charge controller rating</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Short-circuit current. Cannot exceed charge controller rating</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick O'Keeffe:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Battery voltage regulation level.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="213">
   <si>
     <t>Running power</t>
   </si>
@@ -977,15 +1097,6 @@
     <t>Off in stand-by</t>
   </si>
   <si>
-    <t>Mass flow controller</t>
-  </si>
-  <si>
-    <t>MC-20SLPM-D</t>
-  </si>
-  <si>
-    <t>12-30Vdc @ 250mA</t>
-  </si>
-  <si>
     <t>Pump</t>
   </si>
   <si>
@@ -1115,18 +1226,12 @@
     <t>Sun hours per day</t>
   </si>
   <si>
-    <t>Astronergy</t>
-  </si>
-  <si>
     <t>Generation requirement</t>
   </si>
   <si>
     <t>W/hr</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Required # of solar panels</t>
   </si>
   <si>
@@ -1134,9 +1239,6 @@
   </si>
   <si>
     <t>Max amperage to PV controller</t>
-  </si>
-  <si>
-    <t>Power</t>
   </si>
   <si>
     <t>Watts</t>
@@ -1547,7 +1649,46 @@
     <t>Model</t>
   </si>
   <si>
-    <t>CHSM6610P-255</t>
+    <t>Selected charge controller characteristics</t>
+  </si>
+  <si>
+    <t>Max voltage</t>
+  </si>
+  <si>
+    <t>Regulated at</t>
+  </si>
+  <si>
+    <t>Rated power</t>
+  </si>
+  <si>
+    <t>Actual power</t>
+  </si>
+  <si>
+    <t>Vmp</t>
+  </si>
+  <si>
+    <t>Voc</t>
+  </si>
+  <si>
+    <t>MorningStar Corp.</t>
+  </si>
+  <si>
+    <t>SunSaver SS-10-12V</t>
+  </si>
+  <si>
+    <t>Max amperage</t>
+  </si>
+  <si>
+    <t>Isc</t>
+  </si>
+  <si>
+    <t>Imp</t>
+  </si>
+  <si>
+    <t>Solarland</t>
+  </si>
+  <si>
+    <t>SLP150S-12</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1941,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1988,6 +2129,9 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2009,7 +2153,147 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="4"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2025,6 +2309,146 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -2158,6 +2582,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2391,11 +2816,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236351632"/>
-        <c:axId val="236838112"/>
+        <c:axId val="238243360"/>
+        <c:axId val="237967896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236351632"/>
+        <c:axId val="238243360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2449,6 +2874,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2515,12 +2941,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236838112"/>
+        <c:crossAx val="237967896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236838112"/>
+        <c:axId val="237967896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2566,6 +2992,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2632,7 +3059,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236351632"/>
+        <c:crossAx val="238243360"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3639,76 +4066,76 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="20"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B4" s="19">
         <v>1013</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B5" s="19">
         <v>923</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B6" s="19">
         <v>834</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B11" s="48">
         <v>55</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B12" s="49">
         <v>923</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3736,7 +4163,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25"/>
@@ -3775,34 +4202,34 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B7" s="28">
         <v>6</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B8" s="28">
         <v>33</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B9" s="29">
         <v>0.1</v>
@@ -3810,46 +4237,46 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B10" s="28">
         <v>0.85</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B11" s="28">
         <v>24</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B14" s="30">
         <f>B7*(14.7/(B4/68.947573))*((B3+460)/530)</f>
         <v>6.4020229530019002</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B15" s="31">
         <f>ERF(B10/SQRT(2))</f>
@@ -3858,7 +4285,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B16" s="31">
         <f>(1-B15)/2</f>
@@ -3867,14 +4294,14 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B17" s="32">
         <f>B8*(0.528-B9)*1000/(B14*B16*60*B11)</f>
         <v>7.7509263683374092</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3915,60 +4342,60 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E1" s="34" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="79" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="79"/>
+        <v>144</v>
+      </c>
+      <c r="H1" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="80"/>
       <c r="J1" s="33"/>
       <c r="K1" s="34" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L1" s="33"/>
       <c r="O1" s="33" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I2" s="34" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -4120,7 +4547,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="67">
         <v>2.5</v>
@@ -4164,13 +4591,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B7" s="33">
         <v>7</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E7" s="67">
         <v>3</v>
@@ -4214,10 +4641,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E8" s="67">
         <v>3.5</v>
@@ -4261,14 +4688,14 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B9" s="33">
         <f>0.25-2*0.047</f>
         <v>0.156</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E9" s="67">
         <v>4</v>
@@ -4312,14 +4739,14 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B10" s="33">
         <f>0.25-2*0.062</f>
         <v>0.126</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E10" s="67">
         <v>4.5</v>
@@ -4363,14 +4790,14 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B11" s="33">
         <f>0.125-2*0.047</f>
         <v>3.1E-2</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E11" s="67">
         <v>5</v>
@@ -4455,7 +4882,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E13" s="67">
         <v>6</v>
@@ -4499,13 +4926,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B14" s="67">
         <v>3.1E-2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E14" s="67">
         <v>6.5</v>
@@ -4549,13 +4976,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B15" s="67">
         <v>20</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E15" s="67">
         <v>7</v>
@@ -4599,13 +5026,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B16" s="68">
         <v>50</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E16" s="67">
         <v>7.5</v>
@@ -4649,7 +5076,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B17" s="68">
         <v>4100</v>
@@ -4737,7 +5164,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E19" s="67">
         <v>9</v>
@@ -4781,14 +5208,14 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B20" s="42">
         <f>(B3-32)*5/9</f>
         <v>12.777777777777779</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E20" s="67">
         <v>9.5</v>
@@ -4832,14 +5259,14 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B21" s="43">
         <f>1000*(B4/B38)/(B34*(B20+273.15))</f>
         <v>1.1245420441113285</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E21" s="67">
         <v>10</v>
@@ -4883,14 +5310,14 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B22" s="44">
         <f>B36*(B20+273.15)^1.5/((B20+273.15+B35)*10^6)</f>
         <v>1.8009406563349156E-5</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E22" s="67">
         <v>10.5</v>
@@ -4934,14 +5361,14 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B23" s="45">
         <f>PI()*(B14/2)^2</f>
         <v>7.5476763502494771E-4</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E23" s="67">
         <v>11</v>
@@ -4985,14 +5412,14 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B24" s="66">
         <f>$B$15*$B$23*$B$43*$B$46</f>
         <v>2.9684221296677897</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E24" s="67">
         <v>11.5</v>
@@ -5036,7 +5463,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B25" s="70">
         <f>(B24/B42)/(Canisters!B8*(0.528-Canisters!B9))</f>
@@ -5084,14 +5511,14 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="46" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B26" s="47">
         <f>-1*B7*B39</f>
         <v>-482.58</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E26" s="67">
         <v>12.5</v>
@@ -5135,14 +5562,14 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="46" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B27" s="47">
         <f>-1*(1-$B$37)*$B$4-$B$16</f>
         <v>-485.65599999999995</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E27" s="67">
         <v>13</v>
@@ -5186,14 +5613,14 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B28" s="47">
         <f>$B$4*$B$37</f>
         <v>487.34400000000005</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E28" s="67">
         <v>13.5</v>
@@ -5237,14 +5664,14 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B29" s="47">
         <f>$B$4+MIN($B$26:$B$27)-MAX($O$3:$O$31)</f>
         <v>435.63600101214121</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E29" s="67">
         <v>14</v>
@@ -5288,14 +5715,14 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B30" s="47">
         <f>$B$4*($B$37-Canisters!B9)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E30" s="67">
         <v>14.5</v>
@@ -5339,14 +5766,14 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B31" s="69">
         <f>MIN(B29:B30)</f>
         <v>395.04400000000004</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E31" s="67">
         <v>15</v>
@@ -5390,45 +5817,45 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B34" s="41">
         <v>287.05799999999999</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B35" s="33">
         <v>120</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B36" s="33">
         <v>1.512041288</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B37" s="33">
         <v>0.52800000000000002</v>
@@ -5436,101 +5863,101 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B38" s="33">
         <v>10</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B39" s="33">
         <v>68.94</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B40" s="33">
         <v>39.369999999999997</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B41" s="33">
         <v>60</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B42" s="33">
         <v>1000</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B43" s="33">
         <v>12</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B44" s="33">
         <v>3.2810000000000001</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B45" s="33">
         <v>1000</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B46" s="33">
         <v>16.387063999999999</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5538,7 +5965,7 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>$B$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5553,10 +5980,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5578,8 +6005,8 @@
         <v>0</v>
       </c>
       <c r="I1" s="14">
-        <f>SUM(I5:I28)</f>
-        <v>20.499620540119341</v>
+        <f>SUM(I5:I27)</f>
+        <v>17.511480292706704</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -5620,7 +6047,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>10</v>
@@ -5687,7 +6114,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="50">
-        <f t="shared" ref="I6:I16" si="1">G6*D6*H6</f>
+        <f t="shared" ref="I6:I15" si="1">G6*D6*H6</f>
         <v>0.51600000000000001</v>
       </c>
     </row>
@@ -5899,16 +6326,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D14" s="71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="71">
         <v>5</v>
@@ -5926,7 +6353,7 @@
       </c>
       <c r="I14" s="50">
         <f t="shared" si="1"/>
-        <v>2.3719505174723085E-2</v>
+        <v>3.5579257762084628E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -5934,59 +6361,28 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="D15" s="71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="71">
         <v>12</v>
       </c>
       <c r="F15" s="72">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="G15" s="1">
         <f>E15*F15</f>
-        <v>3</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="H15" s="15">
         <v>1</v>
       </c>
       <c r="I15" s="50">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" t="s">
-        <v>194</v>
-      </c>
-      <c r="D16" s="71">
-        <v>2</v>
-      </c>
-      <c r="E16" s="71">
-        <v>12</v>
-      </c>
-      <c r="F16" s="72">
-        <v>0.4</v>
-      </c>
-      <c r="G16" s="1">
-        <f>E16*F16</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="H16" s="15">
-        <v>1</v>
-      </c>
-      <c r="I16" s="50">
         <f t="shared" si="1"/>
         <v>9.6000000000000014</v>
       </c>
@@ -6007,7 +6403,7 @@
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F22" sqref="F22:G22"/>
@@ -6019,7 +6415,7 @@
     <col min="2" max="2" width="6"/>
     <col min="3" max="3" width="9"/>
     <col min="4" max="4" width="4.42578125"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.140625"/>
@@ -6031,47 +6427,47 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="16">
         <f>Consumption!I1</f>
-        <v>20.499620540119341</v>
+        <v>17.511480292706704</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
+      <c r="E1" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="I1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="16">
         <f>B1/B13</f>
-        <v>1.7083017116766117</v>
+        <v>1.4592900243922253</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G2" s="53"/>
-      <c r="J2" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="80"/>
+      <c r="J2" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="81"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="16">
         <f>Consumption!I2</f>
@@ -6081,22 +6477,22 @@
         <v>1</v>
       </c>
       <c r="E3" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="J3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="K3" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -6117,7 +6513,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J4" s="1">
         <v>4</v>
@@ -6126,7 +6522,7 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -6157,7 +6553,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E7" s="60">
         <v>50</v>
@@ -6173,14 +6569,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="65">
         <f>Canisters!B11</f>
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="60">
@@ -6195,14 +6591,14 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9">
         <f>B8*B1+(24-B8)*B3</f>
-        <v>491.99089296286422</v>
+        <v>420.27552702496087</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="60">
         <v>30</v>
@@ -6227,44 +6623,44 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="10">
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="81" t="s">
-        <v>198</v>
-      </c>
-      <c r="G13" s="81"/>
+        <v>63</v>
+      </c>
+      <c r="F13" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="82"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11">
         <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="7">
         <v>6</v>
@@ -6275,7 +6671,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="12">
         <v>0.5</v>
@@ -6283,19 +6679,19 @@
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="75">
         <f>-116.5*LN(B2)+771.1</f>
-        <v>708.7142819271786</v>
+        <v>727.06882118082081</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16" s="11">
         <v>1.59</v>
@@ -6303,279 +6699,371 @@
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" s="13">
         <f>(B9*B14*B16)/(B13*B15)</f>
-        <v>1303.7758663515901</v>
+        <v>1113.7301466161464</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F17" s="14">
         <f>F15*F16*(F14/B13)</f>
-        <v>1417.4285638543572</v>
+        <v>1454.1376423616416</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" s="14">
         <f>IF(F14&lt;12, EVEN((B17/F15)*(B13/F14)), CEILING((B17/F15)*(B13/F14),1))</f>
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B21" s="11">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
-      </c>
-      <c r="F21" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="82"/>
+        <v>197</v>
+      </c>
+      <c r="F21" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="G21" s="83"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B22" s="14">
         <f>$B$9/B21</f>
-        <v>122.99772324071606</v>
+        <v>105.06888175624022</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
-      </c>
-      <c r="F22" s="81" t="s">
-        <v>205</v>
-      </c>
-      <c r="G22" s="81"/>
+        <v>198</v>
+      </c>
+      <c r="F22" s="82" t="s">
+        <v>212</v>
+      </c>
+      <c r="G22" s="82"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1">
-        <f>CEILING(B22/F25,1)</f>
+        <f>CEILING(B22/F28,1)</f>
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="F23" s="7">
-        <v>8.33</v>
+        <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B24" s="14">
-        <f>B23*F23</f>
-        <v>8.33</v>
+        <f>B23*F24</f>
+        <v>8.34</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>210</v>
       </c>
       <c r="F24" s="7">
-        <v>30.68</v>
+        <v>8.34</v>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="1">
-        <f>ROUND(F24*F23, 0)</f>
-        <v>256</v>
+        <v>205</v>
+      </c>
+      <c r="F25" s="79">
+        <v>21.6</v>
       </c>
       <c r="G25" t="s">
-        <v>91</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>209</v>
+      </c>
+      <c r="F26" s="79">
+        <v>9.17</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>199</v>
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>202</v>
+      </c>
+      <c r="F27" s="1">
+        <f>ROUND(F23*F24, 0)</f>
+        <v>150</v>
+      </c>
+      <c r="G27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="11">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="B28" s="14">
+        <f>$B$9/B27</f>
+        <v>210.13776351248043</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="76" t="s">
-        <v>200</v>
-      </c>
-      <c r="F28" s="78">
-        <v>0.2</v>
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28" s="14">
+        <f>F24*F35</f>
+        <v>120.096</v>
+      </c>
+      <c r="G28" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="14">
-        <f>$B$9/B28</f>
-        <v>245.99544648143211</v>
+        <v>82</v>
+      </c>
+      <c r="B29" s="1">
+        <f>CEILING(B28/F28,1)</f>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="77" t="s">
-        <v>202</v>
-      </c>
-      <c r="F29" s="14">
-        <f>B24/(1-F28)</f>
-        <v>10.4125</v>
-      </c>
-      <c r="G29" s="76" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="14">
+        <f>B29*F24</f>
+        <v>16.68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="G31" s="83"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="83" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="83"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" t="s">
+        <v>208</v>
+      </c>
+      <c r="F33" s="79">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="79">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="77" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="14">
+        <f>B24/(1-B34)</f>
+        <v>10.424999999999999</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="79">
+        <v>14.4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="76" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" s="14">
+        <f>B30/(1-B34)</f>
+        <v>20.849999999999998</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="1">
-        <f>CEILING(B29/F25,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E38" s="76"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="76"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="F30" s="14">
-        <f>B31/(1-F28)</f>
-        <v>10.4125</v>
-      </c>
-      <c r="G30" s="76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B39" s="1">
+        <f>F23</f>
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="14">
-        <f>B30*F23</f>
-        <v>8.33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="1">
-        <f>F24</f>
-        <v>30.68</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F13:G13"/>
@@ -6583,24 +7071,50 @@
     <mergeCell ref="F21:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
       <formula>$B$17</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
+      <formula>$F$34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="lessThan">
+      <formula>$F$35*1.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30 B24">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+      <formula>$F$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+      <formula>$F$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$F$33</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A40" r:id="rId1" display="http://rimstar.org/renewnrg/sizing_select_batteries_for_off_grid_solar_system.htm"/>
-    <hyperlink ref="A41" r:id="rId2" display="http://pdf.wholesalesolar.com/Download%20folder/System_Worksheet.pdf"/>
-    <hyperlink ref="A42" r:id="rId3" display="http://rimstar.org/renewnrg/solar_voltage_drop_table_calculator_wire_sizing_for_dc.htm"/>
-    <hyperlink ref="A43" r:id="rId4" display="http://pvwatts.nrel.gov/pvwatts.php"/>
-    <hyperlink ref="A44" r:id="rId5" display="http://www.ecy.wa.gov/climatechange/maps/solar/solar_state.pdf"/>
-    <hyperlink ref="A45" r:id="rId6" display="http://www.nrel.gov/gis/images/map_pv_national_hi-res_200.jpg"/>
+    <hyperlink ref="A42" r:id="rId1" display="http://rimstar.org/renewnrg/sizing_select_batteries_for_off_grid_solar_system.htm"/>
+    <hyperlink ref="A43" r:id="rId2" display="http://pdf.wholesalesolar.com/Download%20folder/System_Worksheet.pdf"/>
+    <hyperlink ref="A44" r:id="rId3" display="http://rimstar.org/renewnrg/solar_voltage_drop_table_calculator_wire_sizing_for_dc.htm"/>
+    <hyperlink ref="A45" r:id="rId4" display="http://pvwatts.nrel.gov/pvwatts.php"/>
+    <hyperlink ref="A46" r:id="rId5" display="http://www.ecy.wa.gov/climatechange/maps/solar/solar_state.pdf"/>
+    <hyperlink ref="A47" r:id="rId6" display="http://www.nrel.gov/gis/images/map_pv_national_hi-res_200.jpg"/>
   </hyperlinks>
   <pageMargins left="1.5" right="1.5" top="2.2374999999999998" bottom="2.2374999999999998" header="2" footer="2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -6620,13 +7134,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B1" s="73" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FIX: separate valve control relays from pump relays in power calcs
The valve control relays operate at 20% duty level but pump relay runs
all the time while in sampling mode. Impact on power consumption is
negligible.
</commit_message>
<xml_diff>
--- a/engr/calculations.xlsx
+++ b/engr/calculations.xlsx
@@ -984,7 +984,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="214">
   <si>
     <t>Running power</t>
   </si>
@@ -1689,6 +1689,9 @@
   </si>
   <si>
     <t>SLP150S-12</t>
+  </si>
+  <si>
+    <t>Pump control relay</t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1944,7 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2132,17 +2135,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2153,97 +2159,7 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="4"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2309,146 +2225,6 @@
         <sz val="11"/>
         <color rgb="FF9C0006"/>
         <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -2582,7 +2358,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2816,11 +2591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238243360"/>
-        <c:axId val="237967896"/>
+        <c:axId val="239147712"/>
+        <c:axId val="239148096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238243360"/>
+        <c:axId val="239147712"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2874,7 +2649,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2941,12 +2715,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237967896"/>
+        <c:crossAx val="239148096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237967896"/>
+        <c:axId val="239148096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2992,7 +2766,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3059,7 +2832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238243360"/>
+        <c:crossAx val="239147712"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4350,10 +4123,10 @@
       <c r="G1" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="80" t="s">
+      <c r="H1" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="80"/>
+      <c r="I1" s="81"/>
       <c r="J1" s="33"/>
       <c r="K1" s="34" t="s">
         <v>171</v>
@@ -5965,7 +5738,7 @@
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J31">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
       <formula>$B$17</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5980,10 +5753,10 @@
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6006,7 +5779,7 @@
       </c>
       <c r="I1" s="14">
         <f>SUM(I5:I27)</f>
-        <v>17.511480292706704</v>
+        <v>17.55962054011934</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -6277,17 +6050,8 @@
       <c r="D12" s="71"/>
       <c r="E12" s="71"/>
       <c r="F12" s="72"/>
-      <c r="G12" s="1">
-        <f t="shared" ref="G12" si="2">E12*F12</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="15">
-        <v>1</v>
-      </c>
-      <c r="I12" s="50">
-        <f t="shared" ref="I12" si="3">G12*D12*H12</f>
-        <v>0</v>
-      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="50"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -6335,7 +6099,7 @@
         <v>189</v>
       </c>
       <c r="D14" s="71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="71">
         <v>5</v>
@@ -6353,37 +6117,68 @@
       </c>
       <c r="I14" s="50">
         <f t="shared" si="1"/>
-        <v>3.5579257762084628E-2</v>
+        <v>2.3719505174723085E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="71">
-        <v>2</v>
-      </c>
-      <c r="E15" s="71">
-        <v>12</v>
+        <v>189</v>
+      </c>
+      <c r="D15" s="80">
+        <v>1</v>
+      </c>
+      <c r="E15" s="80">
+        <v>5</v>
       </c>
       <c r="F15" s="72">
-        <v>0.4</v>
+        <v>1.2E-2</v>
       </c>
       <c r="G15" s="1">
         <f>E15*F15</f>
-        <v>4.8000000000000007</v>
+        <v>0.06</v>
       </c>
       <c r="H15" s="15">
         <v>1</v>
       </c>
       <c r="I15" s="50">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I15" si="2">G15*D15*H15</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="71">
+        <v>2</v>
+      </c>
+      <c r="E16" s="71">
+        <v>12</v>
+      </c>
+      <c r="F16" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="G16" s="1">
+        <f>E16*F16</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="50">
+        <f>G16*D16*H16</f>
         <v>9.6000000000000014</v>
       </c>
     </row>
@@ -6406,7 +6201,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:G22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6431,16 +6226,16 @@
       </c>
       <c r="B1" s="16">
         <f>Consumption!I1</f>
-        <v>17.511480292706704</v>
+        <v>17.55962054011934</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="I1" s="4" t="s">
         <v>42</v>
       </c>
@@ -6448,7 +6243,7 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="16">
         <f>B1/B13</f>
-        <v>1.4592900243922253</v>
+        <v>1.4633017116766116</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -6460,10 +6255,10 @@
         <v>43</v>
       </c>
       <c r="G2" s="53"/>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="81"/>
+      <c r="K2" s="83"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -6595,7 +6390,7 @@
       </c>
       <c r="B9" s="9">
         <f>B8*B1+(24-B8)*B3</f>
-        <v>420.27552702496087</v>
+        <v>421.43089296286416</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>58</v>
@@ -6643,10 +6438,10 @@
       <c r="E13" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="G13" s="82"/>
+      <c r="G13" s="84"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -6683,7 +6478,7 @@
       </c>
       <c r="F15" s="75">
         <f>-116.5*LN(B2)+771.1</f>
-        <v>727.06882118082081</v>
+        <v>726.74899418864027</v>
       </c>
       <c r="G15" t="s">
         <v>69</v>
@@ -6714,7 +6509,7 @@
       </c>
       <c r="B17" s="13">
         <f>(B9*B14*B16)/(B13*B15)</f>
-        <v>1113.7301466161464</v>
+        <v>1116.79186635159</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>74</v>
@@ -6725,7 +6520,7 @@
       </c>
       <c r="F17" s="14">
         <f>F15*F16*(F14/B13)</f>
-        <v>1454.1376423616416</v>
+        <v>1453.4979883772805</v>
       </c>
       <c r="G17" t="s">
         <v>69</v>
@@ -6764,10 +6559,10 @@
       <c r="E21" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="83" t="s">
+      <c r="F21" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="G21" s="83"/>
+      <c r="G21" s="82"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -6775,7 +6570,7 @@
       </c>
       <c r="B22" s="14">
         <f>$B$9/B21</f>
-        <v>105.06888175624022</v>
+        <v>105.35772324071604</v>
       </c>
       <c r="C22" t="s">
         <v>81</v>
@@ -6783,10 +6578,10 @@
       <c r="E22" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="82" t="s">
+      <c r="F22" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="G22" s="82"/>
+      <c r="G22" s="84"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -6882,7 +6677,7 @@
       </c>
       <c r="B28" s="14">
         <f>$B$9/B27</f>
-        <v>210.13776351248043</v>
+        <v>210.71544648143208</v>
       </c>
       <c r="C28" t="s">
         <v>81</v>
@@ -6929,19 +6724,19 @@
       <c r="E31" t="s">
         <v>197</v>
       </c>
-      <c r="F31" s="83" t="s">
+      <c r="F31" s="82" t="s">
         <v>206</v>
       </c>
-      <c r="G31" s="83"/>
+      <c r="G31" s="82"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>198</v>
       </c>
-      <c r="F32" s="83" t="s">
+      <c r="F32" s="82" t="s">
         <v>207</v>
       </c>
-      <c r="G32" s="83"/>
+      <c r="G32" s="82"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
@@ -7071,27 +6866,27 @@
     <mergeCell ref="F21:G21"/>
   </mergeCells>
   <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>$B$17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="greaterThan">
       <formula>$F$34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
       <formula>$F$35*1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30 B24">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="greaterThan">
       <formula>$F$33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$F$33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>